<commit_message>
SW roster pdf updated
</commit_message>
<xml_diff>
--- a/secure/club-roster2019.xlsx
+++ b/secure/club-roster2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9CB92F-B250-46ED-BBBF-6EB3B098E955}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0594A625-DA7E-445C-BA60-8C8848F0A71C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="3690" windowWidth="19890" windowHeight="11835" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
+    <workbookView xWindow="8250" yWindow="1140" windowWidth="18195" windowHeight="11820" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2663,14 +2663,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3094,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EEE842-FA9A-4617-9438-69514D1A7666}">
   <dimension ref="A1:D343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G145" sqref="G145"/>
+    <sheetView tabSelected="1" topLeftCell="A324" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,10 +3108,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>730</v>
       </c>
-      <c r="C1" s="64"/>
+      <c r="C1" s="65"/>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4704,7 +4704,7 @@
       <c r="B138" s="44" t="s">
         <v>728</v>
       </c>
-      <c r="C138" s="65" t="s">
+      <c r="C138" s="63" t="s">
         <v>735</v>
       </c>
       <c r="D138" s="53">

</xml_diff>

<commit_message>
SW fixed a couple of contacts
</commit_message>
<xml_diff>
--- a/secure/club-roster2019.xlsx
+++ b/secure/club-roster2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0594A625-DA7E-445C-BA60-8C8848F0A71C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F0CBC4-28F5-482B-BDE5-443A265656B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="1140" windowWidth="18195" windowHeight="11820" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
+    <workbookView xWindow="3510" yWindow="690" windowWidth="18225" windowHeight="15510" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="745">
   <si>
     <t>Beach Grove Golf Club</t>
   </si>
@@ -586,9 +586,6 @@
     <t>604-983-9455</t>
   </si>
   <si>
-    <t>wilma.macmillan@gmail.com</t>
-  </si>
-  <si>
     <t>Glen Eagles</t>
   </si>
   <si>
@@ -2258,6 +2255,15 @@
   </si>
   <si>
     <t>gena.mcc@gmail.com</t>
+  </si>
+  <si>
+    <t>wilma.macmillan@ymail.com</t>
+  </si>
+  <si>
+    <t>Joanne Webster</t>
+  </si>
+  <si>
+    <t>jmelloywebster@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2525,7 +2531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2671,6 +2677,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3092,10 +3102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EEE842-FA9A-4617-9438-69514D1A7666}">
-  <dimension ref="A1:D343"/>
+  <dimension ref="A1:F343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D343"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D343" sqref="A1:D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,7 +3119,7 @@
     <row r="1" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="64" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C1" s="65"/>
       <c r="D1"/>
@@ -3867,7 +3877,7 @@
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="5"/>
@@ -4027,195 +4037,196 @@
       <c r="C80" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="D80" s="40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="67" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
       <c r="D81" s="11"/>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F81" s="66"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B83" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C83" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="C83" s="32" t="s">
+      <c r="D83" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="D83" s="33" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="31" t="s">
         <v>22</v>
       </c>
       <c r="B84" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C84" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C84" s="32" t="s">
+      <c r="D84" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="D84" s="33" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="31" t="s">
         <v>5</v>
       </c>
       <c r="B85" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C85" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="C85" s="32" t="s">
+      <c r="D85" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="D85" s="33" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B86" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="C86" s="32" t="s">
+      <c r="D86" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="D86" s="33" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="31" t="s">
         <v>11</v>
       </c>
       <c r="B87" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="C87" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="C87" s="32" t="s">
+      <c r="D87" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D87" s="33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B88" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C88" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="D88" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="D88" s="33" t="s">
+    </row>
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B91" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="D91" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="D91" s="27" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B92" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="C92" s="26" t="s">
+      <c r="D92" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="D92" s="27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B93" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C93" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="C93" s="26" t="s">
+      <c r="D93" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="D93" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B94" s="26" t="s">
+        <v>214</v>
+      </c>
+      <c r="C94" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="C94" s="26" t="s">
+      <c r="D94" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="D94" s="27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B95" s="26" t="s">
+        <v>217</v>
+      </c>
+      <c r="C95" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="C95" s="26" t="s">
+      <c r="D95" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="D95" s="27" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B96" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C96" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C96" s="26" t="s">
+      <c r="D96" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="D96" s="27" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4223,13 +4234,13 @@
         <v>72</v>
       </c>
       <c r="B97" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C97" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C97" s="26" t="s">
+      <c r="D97" s="27" t="s">
         <v>225</v>
-      </c>
-      <c r="D97" s="27" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4237,13 +4248,13 @@
         <v>48</v>
       </c>
       <c r="B98" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C98" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C98" s="26" t="s">
+      <c r="D98" s="27" t="s">
         <v>222</v>
-      </c>
-      <c r="D98" s="27" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,7 +4262,7 @@
     </row>
     <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="5"/>
@@ -4261,13 +4272,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="C101" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="C101" s="32" t="s">
+      <c r="D101" s="33" t="s">
         <v>229</v>
-      </c>
-      <c r="D101" s="33" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,13 +4286,13 @@
         <v>22</v>
       </c>
       <c r="B102" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="C102" s="32" t="s">
+      <c r="D102" s="33" t="s">
         <v>232</v>
-      </c>
-      <c r="D102" s="33" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4289,13 +4300,13 @@
         <v>5</v>
       </c>
       <c r="B103" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="C103" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="D103" s="33" t="s">
         <v>235</v>
-      </c>
-      <c r="D103" s="33" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4303,13 +4314,13 @@
         <v>8</v>
       </c>
       <c r="B104" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="C104" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="C104" s="32" t="s">
+      <c r="D104" s="33" t="s">
         <v>238</v>
-      </c>
-      <c r="D104" s="33" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4317,13 +4328,13 @@
         <v>11</v>
       </c>
       <c r="B105" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="C105" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="C105" s="32" t="s">
+      <c r="D105" s="33" t="s">
         <v>241</v>
-      </c>
-      <c r="D105" s="33" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,13 +4342,13 @@
         <v>14</v>
       </c>
       <c r="B106" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="C106" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="D106" s="33" t="s">
         <v>244</v>
-      </c>
-      <c r="D106" s="33" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4345,13 +4356,13 @@
         <v>72</v>
       </c>
       <c r="B107" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="C107" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="D107" s="33" t="s">
         <v>238</v>
-      </c>
-      <c r="D107" s="33" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4359,13 +4370,13 @@
         <v>48</v>
       </c>
       <c r="B108" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="C108" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="C108" s="32" t="s">
+      <c r="D108" s="33" t="s">
         <v>247</v>
-      </c>
-      <c r="D108" s="33" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4375,7 +4386,7 @@
     </row>
     <row r="110" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -4386,13 +4397,13 @@
         <v>1</v>
       </c>
       <c r="B111" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C111" s="39" t="s">
         <v>250</v>
       </c>
-      <c r="C111" s="39" t="s">
+      <c r="D111" s="40" t="s">
         <v>251</v>
-      </c>
-      <c r="D111" s="40" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4400,13 +4411,13 @@
         <v>22</v>
       </c>
       <c r="B112" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="C112" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="C112" s="39" t="s">
+      <c r="D112" s="40" t="s">
         <v>254</v>
-      </c>
-      <c r="D112" s="40" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4414,13 +4425,13 @@
         <v>5</v>
       </c>
       <c r="B113" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="C113" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="C113" s="39" t="s">
+      <c r="D113" s="40" t="s">
         <v>257</v>
-      </c>
-      <c r="D113" s="40" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4428,27 +4439,27 @@
         <v>8</v>
       </c>
       <c r="B114" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="C114" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="C114" s="39" t="s">
+      <c r="D114" s="40" t="s">
         <v>260</v>
-      </c>
-      <c r="D114" s="40" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="B115" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="B115" s="39" t="s">
+      <c r="C115" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="C115" s="39" t="s">
+      <c r="D115" s="40" t="s">
         <v>264</v>
-      </c>
-      <c r="D115" s="40" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4456,18 +4467,18 @@
         <v>14</v>
       </c>
       <c r="B116" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="C116" s="39" t="s">
         <v>266</v>
       </c>
-      <c r="C116" s="39" t="s">
+      <c r="D116" s="40" t="s">
         <v>267</v>
-      </c>
-      <c r="D116" s="40" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="5"/>
@@ -4477,13 +4488,13 @@
         <v>1</v>
       </c>
       <c r="B119" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="C119" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="C119" s="26" t="s">
+      <c r="D119" s="27" t="s">
         <v>271</v>
-      </c>
-      <c r="D119" s="27" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,13 +4502,13 @@
         <v>22</v>
       </c>
       <c r="B120" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="C120" s="26" t="s">
         <v>273</v>
       </c>
-      <c r="C120" s="26" t="s">
+      <c r="D120" s="27" t="s">
         <v>274</v>
-      </c>
-      <c r="D120" s="27" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4505,13 +4516,13 @@
         <v>5</v>
       </c>
       <c r="B121" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="C121" s="26" t="s">
         <v>276</v>
       </c>
-      <c r="C121" s="26" t="s">
+      <c r="D121" s="27" t="s">
         <v>277</v>
-      </c>
-      <c r="D121" s="27" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4519,13 +4530,13 @@
         <v>8</v>
       </c>
       <c r="B122" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C122" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="C122" s="26" t="s">
+      <c r="D122" s="27" t="s">
         <v>280</v>
-      </c>
-      <c r="D122" s="27" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4533,13 +4544,13 @@
         <v>11</v>
       </c>
       <c r="B123" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="C123" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="C123" s="26" t="s">
+      <c r="D123" s="27" t="s">
         <v>283</v>
-      </c>
-      <c r="D123" s="27" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4547,13 +4558,13 @@
         <v>14</v>
       </c>
       <c r="B124" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C124" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="C124" s="26" t="s">
+      <c r="D124" s="41" t="s">
         <v>286</v>
-      </c>
-      <c r="D124" s="41" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4561,13 +4572,13 @@
         <v>72</v>
       </c>
       <c r="B125" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="C125" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="C125" s="26" t="s">
+      <c r="D125" s="27" t="s">
         <v>289</v>
-      </c>
-      <c r="D125" s="27" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4575,13 +4586,13 @@
         <v>48</v>
       </c>
       <c r="B126" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C126" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="C126" s="26" t="s">
+      <c r="D126" s="27" t="s">
         <v>292</v>
-      </c>
-      <c r="D126" s="27" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4589,7 +4600,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D128" s="6"/>
     </row>
@@ -4598,13 +4609,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="C129" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="C129" s="26" t="s">
+      <c r="D129" s="26" t="s">
         <v>296</v>
-      </c>
-      <c r="D129" s="26" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4612,13 +4623,13 @@
         <v>22</v>
       </c>
       <c r="B130" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="C130" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="C130" s="26" t="s">
+      <c r="D130" s="26" t="s">
         <v>299</v>
-      </c>
-      <c r="D130" s="26" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,7 +4637,7 @@
         <v>5</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C131" s="26"/>
       <c r="D131" s="27"/>
@@ -4636,13 +4647,13 @@
         <v>8</v>
       </c>
       <c r="B132" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C132" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="C132" s="26" t="s">
+      <c r="D132" s="26" t="s">
         <v>303</v>
-      </c>
-      <c r="D132" s="26" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4650,13 +4661,13 @@
         <v>11</v>
       </c>
       <c r="B133" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="C133" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="C133" s="26" t="s">
+      <c r="D133" s="26" t="s">
         <v>306</v>
-      </c>
-      <c r="D133" s="26" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4665,7 +4676,7 @@
     </row>
     <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -4673,28 +4684,28 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>730</v>
+      </c>
+      <c r="C136" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="B136" s="32" t="s">
+      <c r="D136" s="33" t="s">
         <v>731</v>
-      </c>
-      <c r="C136" s="42" t="s">
-        <v>310</v>
-      </c>
-      <c r="D136" s="33" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="26"/>
       <c r="B137" s="32" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C137" s="43">
         <v>0</v>
       </c>
       <c r="D137" s="33" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4702,10 +4713,10 @@
         <v>8</v>
       </c>
       <c r="B138" s="44" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C138" s="63" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D138" s="53">
         <v>0</v>
@@ -4714,7 +4725,7 @@
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="50"/>
       <c r="B139" s="51" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C139" s="52"/>
       <c r="D139" s="54"/>
@@ -4722,7 +4733,7 @@
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="45"/>
       <c r="B140" s="46" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C140" s="47"/>
       <c r="D140" s="48"/>
@@ -4732,11 +4743,11 @@
         <v>8</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C141" s="39"/>
       <c r="D141" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4744,11 +4755,11 @@
         <v>11</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C142" s="39"/>
       <c r="D142" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4756,11 +4767,11 @@
         <v>14</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C143" s="39"/>
       <c r="D143" s="33" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4768,45 +4779,45 @@
         <v>15</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C144" s="26"/>
       <c r="D144" s="33" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B145" s="32"/>
       <c r="C145" s="26"/>
       <c r="D145" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C146" s="26"/>
       <c r="D146" s="33" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C147" s="26"/>
       <c r="D147" s="33" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4815,7 +4826,7 @@
     </row>
     <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D149" s="7"/>
     </row>
@@ -4824,13 +4835,13 @@
         <v>1</v>
       </c>
       <c r="B150" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="C150" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="C150" s="26" t="s">
+      <c r="D150" s="27" t="s">
         <v>317</v>
-      </c>
-      <c r="D150" s="27" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4839,7 +4850,7 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="5"/>
@@ -4849,13 +4860,13 @@
         <v>1</v>
       </c>
       <c r="B153" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="C153" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="C153" s="32" t="s">
+      <c r="D153" s="33" t="s">
         <v>320</v>
-      </c>
-      <c r="D153" s="33" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4863,13 +4874,13 @@
         <v>22</v>
       </c>
       <c r="B154" s="39" t="s">
+        <v>321</v>
+      </c>
+      <c r="C154" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="C154" s="39" t="s">
+      <c r="D154" s="40" t="s">
         <v>323</v>
-      </c>
-      <c r="D154" s="40" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4877,13 +4888,13 @@
         <v>5</v>
       </c>
       <c r="B155" s="39" t="s">
+        <v>324</v>
+      </c>
+      <c r="C155" s="39" t="s">
         <v>325</v>
       </c>
-      <c r="C155" s="39" t="s">
+      <c r="D155" s="40" t="s">
         <v>326</v>
-      </c>
-      <c r="D155" s="40" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4891,13 +4902,13 @@
         <v>8</v>
       </c>
       <c r="B156" s="39" t="s">
+        <v>327</v>
+      </c>
+      <c r="C156" s="39" t="s">
         <v>328</v>
       </c>
-      <c r="C156" s="39" t="s">
+      <c r="D156" s="40" t="s">
         <v>329</v>
-      </c>
-      <c r="D156" s="40" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4905,13 +4916,13 @@
         <v>11</v>
       </c>
       <c r="B157" s="39" t="s">
+        <v>330</v>
+      </c>
+      <c r="C157" s="39" t="s">
         <v>331</v>
       </c>
-      <c r="C157" s="39" t="s">
+      <c r="D157" s="40" t="s">
         <v>332</v>
-      </c>
-      <c r="D157" s="40" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4919,13 +4930,13 @@
         <v>14</v>
       </c>
       <c r="B158" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="C158" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="C158" s="39" t="s">
+      <c r="D158" s="40" t="s">
         <v>335</v>
-      </c>
-      <c r="D158" s="40" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4933,25 +4944,25 @@
         <v>72</v>
       </c>
       <c r="B159" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C159" s="39" t="s">
         <v>337</v>
       </c>
-      <c r="C159" s="39" t="s">
+      <c r="D159" s="40" t="s">
         <v>338</v>
-      </c>
-      <c r="D159" s="40" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="26"/>
       <c r="B160" s="39" t="s">
+        <v>339</v>
+      </c>
+      <c r="C160" s="39" t="s">
         <v>340</v>
       </c>
-      <c r="C160" s="39" t="s">
+      <c r="D160" s="40" t="s">
         <v>341</v>
-      </c>
-      <c r="D160" s="40" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4959,13 +4970,13 @@
         <v>48</v>
       </c>
       <c r="B161" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="C161" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="C161" s="39" t="s">
+      <c r="D161" s="40" t="s">
         <v>344</v>
-      </c>
-      <c r="D161" s="40" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4975,7 +4986,7 @@
     </row>
     <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="14"/>
@@ -4986,13 +4997,13 @@
         <v>1</v>
       </c>
       <c r="B164" s="39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C164" s="39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D164" s="40" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -5000,13 +5011,13 @@
         <v>179</v>
       </c>
       <c r="B165" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="C165" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="C165" s="39" t="s">
+      <c r="D165" s="40" t="s">
         <v>349</v>
-      </c>
-      <c r="D165" s="40" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5014,13 +5025,13 @@
         <v>5</v>
       </c>
       <c r="B166" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="C166" s="39" t="s">
         <v>351</v>
       </c>
-      <c r="C166" s="39" t="s">
+      <c r="D166" s="40" t="s">
         <v>352</v>
-      </c>
-      <c r="D166" s="40" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,7 +5041,7 @@
     </row>
     <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="5"/>
@@ -5040,13 +5051,13 @@
         <v>1</v>
       </c>
       <c r="B169" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="C169" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="C169" s="32" t="s">
+      <c r="D169" s="55" t="s">
         <v>356</v>
-      </c>
-      <c r="D169" s="55" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -5054,13 +5065,13 @@
         <v>22</v>
       </c>
       <c r="B170" s="39" t="s">
+        <v>357</v>
+      </c>
+      <c r="C170" s="39" t="s">
         <v>358</v>
       </c>
-      <c r="C170" s="39" t="s">
+      <c r="D170" s="56" t="s">
         <v>359</v>
-      </c>
-      <c r="D170" s="56" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5068,11 +5079,11 @@
         <v>5</v>
       </c>
       <c r="B171" s="39" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C171" s="39"/>
       <c r="D171" s="56" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5080,13 +5091,13 @@
         <v>8</v>
       </c>
       <c r="B172" s="39" t="s">
+        <v>362</v>
+      </c>
+      <c r="C172" s="39" t="s">
         <v>363</v>
       </c>
-      <c r="C172" s="39" t="s">
+      <c r="D172" s="56" t="s">
         <v>364</v>
-      </c>
-      <c r="D172" s="56" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,13 +5105,13 @@
         <v>11</v>
       </c>
       <c r="B173" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="C173" s="39" t="s">
         <v>366</v>
       </c>
-      <c r="C173" s="39" t="s">
+      <c r="D173" s="56" t="s">
         <v>367</v>
-      </c>
-      <c r="D173" s="56" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5108,13 +5119,13 @@
         <v>14</v>
       </c>
       <c r="B174" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="C174" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="C174" s="39" t="s">
+      <c r="D174" s="56" t="s">
         <v>370</v>
-      </c>
-      <c r="D174" s="56" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -5122,13 +5133,13 @@
         <v>48</v>
       </c>
       <c r="B175" s="39" t="s">
+        <v>371</v>
+      </c>
+      <c r="C175" s="39" t="s">
         <v>372</v>
       </c>
-      <c r="C175" s="39" t="s">
+      <c r="D175" s="36" t="s">
         <v>373</v>
-      </c>
-      <c r="D175" s="36" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -5138,7 +5149,7 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B177" s="2"/>
       <c r="D177" s="7"/>
@@ -5148,13 +5159,13 @@
         <v>1</v>
       </c>
       <c r="B178" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="C178" s="26" t="s">
         <v>376</v>
       </c>
-      <c r="C178" s="26" t="s">
+      <c r="D178" s="27" t="s">
         <v>377</v>
-      </c>
-      <c r="D178" s="27" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -5162,13 +5173,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C179" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="C179" s="26" t="s">
+      <c r="D179" s="27" t="s">
         <v>380</v>
-      </c>
-      <c r="D179" s="27" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -5176,13 +5187,13 @@
         <v>5</v>
       </c>
       <c r="B180" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="C180" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="C180" s="26" t="s">
+      <c r="D180" s="27" t="s">
         <v>383</v>
-      </c>
-      <c r="D180" s="27" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -5190,13 +5201,13 @@
         <v>8</v>
       </c>
       <c r="B181" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="C181" s="26" t="s">
         <v>385</v>
       </c>
-      <c r="C181" s="26" t="s">
+      <c r="D181" s="27" t="s">
         <v>386</v>
-      </c>
-      <c r="D181" s="27" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -5204,13 +5215,13 @@
         <v>11</v>
       </c>
       <c r="B182" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="C182" s="26" t="s">
         <v>388</v>
       </c>
-      <c r="C182" s="26" t="s">
+      <c r="D182" s="27" t="s">
         <v>389</v>
-      </c>
-      <c r="D182" s="27" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -5218,13 +5229,13 @@
         <v>14</v>
       </c>
       <c r="B183" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C183" s="26" t="s">
         <v>391</v>
       </c>
-      <c r="C183" s="26" t="s">
+      <c r="D183" s="28" t="s">
         <v>392</v>
-      </c>
-      <c r="D183" s="28" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5234,7 +5245,7 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="5"/>
@@ -5244,27 +5255,27 @@
         <v>1</v>
       </c>
       <c r="B186" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="C186" s="26" t="s">
         <v>395</v>
       </c>
-      <c r="C186" s="26" t="s">
+      <c r="D186" s="27" t="s">
         <v>396</v>
-      </c>
-      <c r="D186" s="27" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="B187" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="B187" s="26" t="s">
+      <c r="C187" s="26" t="s">
         <v>399</v>
       </c>
-      <c r="C187" s="26" t="s">
+      <c r="D187" s="27" t="s">
         <v>400</v>
-      </c>
-      <c r="D187" s="27" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5272,13 +5283,13 @@
         <v>5</v>
       </c>
       <c r="B188" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="C188" s="26" t="s">
         <v>402</v>
       </c>
-      <c r="C188" s="26" t="s">
+      <c r="D188" s="27" t="s">
         <v>403</v>
-      </c>
-      <c r="D188" s="27" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5286,13 +5297,13 @@
         <v>8</v>
       </c>
       <c r="B189" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="C189" s="26" t="s">
         <v>405</v>
       </c>
-      <c r="C189" s="26" t="s">
+      <c r="D189" s="27" t="s">
         <v>406</v>
-      </c>
-      <c r="D189" s="27" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5300,13 +5311,13 @@
         <v>11</v>
       </c>
       <c r="B190" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="C190" s="26" t="s">
         <v>408</v>
       </c>
-      <c r="C190" s="26" t="s">
+      <c r="D190" s="27" t="s">
         <v>409</v>
-      </c>
-      <c r="D190" s="27" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5314,13 +5325,13 @@
         <v>14</v>
       </c>
       <c r="B191" s="26" t="s">
+        <v>410</v>
+      </c>
+      <c r="C191" s="26" t="s">
         <v>411</v>
       </c>
-      <c r="C191" s="26" t="s">
+      <c r="D191" s="27" t="s">
         <v>412</v>
-      </c>
-      <c r="D191" s="27" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5328,18 +5339,18 @@
         <v>48</v>
       </c>
       <c r="B192" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="C192" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="C192" s="26" t="s">
+      <c r="D192" s="27" t="s">
         <v>415</v>
-      </c>
-      <c r="D192" s="27" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="5"/>
@@ -5349,13 +5360,13 @@
         <v>1</v>
       </c>
       <c r="B195" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C195" s="26" t="s">
         <v>418</v>
       </c>
-      <c r="C195" s="26" t="s">
+      <c r="D195" s="27" t="s">
         <v>419</v>
-      </c>
-      <c r="D195" s="27" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5363,13 +5374,13 @@
         <v>22</v>
       </c>
       <c r="B196" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="C196" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="C196" s="26" t="s">
+      <c r="D196" s="27" t="s">
         <v>422</v>
-      </c>
-      <c r="D196" s="27" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5377,13 +5388,13 @@
         <v>5</v>
       </c>
       <c r="B197" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="C197" s="26" t="s">
         <v>424</v>
       </c>
-      <c r="C197" s="26" t="s">
+      <c r="D197" s="27" t="s">
         <v>425</v>
-      </c>
-      <c r="D197" s="27" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5391,13 +5402,13 @@
         <v>8</v>
       </c>
       <c r="B198" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="C198" s="26" t="s">
         <v>427</v>
       </c>
-      <c r="C198" s="26" t="s">
+      <c r="D198" s="27" t="s">
         <v>428</v>
-      </c>
-      <c r="D198" s="27" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5405,18 +5416,18 @@
         <v>14</v>
       </c>
       <c r="B199" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="C199" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="C199" s="26" t="s">
+      <c r="D199" s="27" t="s">
         <v>431</v>
-      </c>
-      <c r="D199" s="27" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
@@ -5426,13 +5437,13 @@
         <v>1</v>
       </c>
       <c r="B202" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="C202" s="26" t="s">
         <v>434</v>
       </c>
-      <c r="C202" s="26" t="s">
+      <c r="D202" s="27" t="s">
         <v>435</v>
-      </c>
-      <c r="D202" s="27" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5440,13 +5451,13 @@
         <v>22</v>
       </c>
       <c r="B203" s="26" t="s">
+        <v>436</v>
+      </c>
+      <c r="C203" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="C203" s="26" t="s">
+      <c r="D203" s="27" t="s">
         <v>438</v>
-      </c>
-      <c r="D203" s="27" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5454,13 +5465,13 @@
         <v>5</v>
       </c>
       <c r="B204" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="C204" s="26" t="s">
         <v>440</v>
       </c>
-      <c r="C204" s="26" t="s">
+      <c r="D204" s="27" t="s">
         <v>441</v>
-      </c>
-      <c r="D204" s="27" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5468,13 +5479,13 @@
         <v>8</v>
       </c>
       <c r="B205" s="26" t="s">
+        <v>442</v>
+      </c>
+      <c r="C205" s="26" t="s">
         <v>443</v>
       </c>
-      <c r="C205" s="26" t="s">
+      <c r="D205" s="27" t="s">
         <v>444</v>
-      </c>
-      <c r="D205" s="27" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5482,13 +5493,13 @@
         <v>11</v>
       </c>
       <c r="B206" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="C206" s="26" t="s">
         <v>446</v>
       </c>
-      <c r="C206" s="26" t="s">
+      <c r="D206" s="27" t="s">
         <v>447</v>
-      </c>
-      <c r="D206" s="27" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5496,13 +5507,13 @@
         <v>14</v>
       </c>
       <c r="B207" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="C207" s="26" t="s">
         <v>446</v>
       </c>
-      <c r="C207" s="26" t="s">
+      <c r="D207" s="27" t="s">
         <v>447</v>
-      </c>
-      <c r="D207" s="27" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5510,7 +5521,7 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D209" s="7"/>
     </row>
@@ -5519,13 +5530,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="C210" s="26" t="s">
         <v>450</v>
       </c>
-      <c r="C210" s="26" t="s">
+      <c r="D210" s="27" t="s">
         <v>451</v>
-      </c>
-      <c r="D210" s="27" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5533,13 +5544,13 @@
         <v>22</v>
       </c>
       <c r="B211" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="C211" s="26" t="s">
         <v>453</v>
       </c>
-      <c r="C211" s="26" t="s">
+      <c r="D211" s="27" t="s">
         <v>454</v>
-      </c>
-      <c r="D211" s="27" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5547,11 +5558,11 @@
         <v>5</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C212" s="26"/>
       <c r="D212" s="27" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5567,11 +5578,11 @@
         <v>14</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C214" s="26"/>
       <c r="D214" s="27" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5579,11 +5590,11 @@
         <v>15</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C215" s="26"/>
       <c r="D215" s="27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5591,13 +5602,13 @@
         <v>68</v>
       </c>
       <c r="B216" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="C216" s="26" t="s">
         <v>462</v>
       </c>
-      <c r="C216" s="26" t="s">
+      <c r="D216" s="27" t="s">
         <v>463</v>
-      </c>
-      <c r="D216" s="27" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5605,13 +5616,13 @@
         <v>72</v>
       </c>
       <c r="B217" s="26" t="s">
+        <v>464</v>
+      </c>
+      <c r="C217" s="26" t="s">
         <v>465</v>
       </c>
-      <c r="C217" s="26" t="s">
+      <c r="D217" s="27" t="s">
         <v>466</v>
-      </c>
-      <c r="D217" s="27" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5619,13 +5630,13 @@
         <v>48</v>
       </c>
       <c r="B218" s="26" t="s">
+        <v>467</v>
+      </c>
+      <c r="C218" s="26" t="s">
         <v>468</v>
       </c>
-      <c r="C218" s="26" t="s">
+      <c r="D218" s="27" t="s">
         <v>469</v>
-      </c>
-      <c r="D218" s="27" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5634,7 +5645,7 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D220" s="7"/>
     </row>
@@ -5643,13 +5654,13 @@
         <v>1</v>
       </c>
       <c r="B221" s="26" t="s">
+        <v>471</v>
+      </c>
+      <c r="C221" s="26" t="s">
         <v>472</v>
       </c>
-      <c r="C221" s="26" t="s">
+      <c r="D221" s="27" t="s">
         <v>473</v>
-      </c>
-      <c r="D221" s="27" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5657,13 +5668,13 @@
         <v>22</v>
       </c>
       <c r="B222" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="C222" s="26" t="s">
         <v>475</v>
       </c>
-      <c r="C222" s="26" t="s">
+      <c r="D222" s="27" t="s">
         <v>476</v>
-      </c>
-      <c r="D222" s="27" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5671,13 +5682,13 @@
         <v>5</v>
       </c>
       <c r="B223" s="26" t="s">
+        <v>477</v>
+      </c>
+      <c r="C223" s="26" t="s">
         <v>478</v>
       </c>
-      <c r="C223" s="26" t="s">
+      <c r="D223" s="27" t="s">
         <v>479</v>
-      </c>
-      <c r="D223" s="27" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5685,13 +5696,13 @@
         <v>8</v>
       </c>
       <c r="B224" s="26" t="s">
+        <v>477</v>
+      </c>
+      <c r="C224" s="26" t="s">
         <v>478</v>
       </c>
-      <c r="C224" s="26" t="s">
+      <c r="D224" s="27" t="s">
         <v>479</v>
-      </c>
-      <c r="D224" s="27" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5699,13 +5710,13 @@
         <v>11</v>
       </c>
       <c r="B225" s="26" t="s">
+        <v>480</v>
+      </c>
+      <c r="C225" s="26" t="s">
         <v>481</v>
       </c>
-      <c r="C225" s="26" t="s">
+      <c r="D225" s="27" t="s">
         <v>482</v>
-      </c>
-      <c r="D225" s="27" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5713,13 +5724,13 @@
         <v>14</v>
       </c>
       <c r="B226" s="26" t="s">
+        <v>480</v>
+      </c>
+      <c r="C226" s="26" t="s">
         <v>481</v>
       </c>
-      <c r="C226" s="26" t="s">
+      <c r="D226" s="27" t="s">
         <v>482</v>
-      </c>
-      <c r="D226" s="27" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5727,13 +5738,13 @@
         <v>68</v>
       </c>
       <c r="B227" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="C227" s="26" t="s">
         <v>484</v>
       </c>
-      <c r="C227" s="26" t="s">
+      <c r="D227" s="27" t="s">
         <v>485</v>
-      </c>
-      <c r="D227" s="27" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5757,13 +5768,13 @@
         <v>107</v>
       </c>
       <c r="B230" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="C230" s="26" t="s">
         <v>475</v>
       </c>
-      <c r="C230" s="26" t="s">
+      <c r="D230" s="57" t="s">
         <v>476</v>
-      </c>
-      <c r="D230" s="57" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5771,7 +5782,7 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B232" s="4"/>
       <c r="C232" s="5"/>
@@ -5781,13 +5792,13 @@
         <v>1</v>
       </c>
       <c r="B233" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="C233" s="26" t="s">
         <v>488</v>
       </c>
-      <c r="C233" s="26" t="s">
+      <c r="D233" s="27" t="s">
         <v>489</v>
-      </c>
-      <c r="D233" s="27" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5795,13 +5806,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="26" t="s">
+        <v>490</v>
+      </c>
+      <c r="C234" s="26" t="s">
         <v>491</v>
       </c>
-      <c r="C234" s="26" t="s">
+      <c r="D234" s="27" t="s">
         <v>492</v>
-      </c>
-      <c r="D234" s="27" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5809,13 +5820,13 @@
         <v>5</v>
       </c>
       <c r="B235" s="26" t="s">
+        <v>493</v>
+      </c>
+      <c r="C235" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="C235" s="26" t="s">
+      <c r="D235" s="27" t="s">
         <v>495</v>
-      </c>
-      <c r="D235" s="27" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5823,11 +5834,11 @@
         <v>8</v>
       </c>
       <c r="B236" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C236" s="26"/>
       <c r="D236" s="27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5843,11 +5854,11 @@
         <v>14</v>
       </c>
       <c r="B238" s="26" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C238" s="26"/>
       <c r="D238" s="27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -5855,11 +5866,11 @@
         <v>15</v>
       </c>
       <c r="B239" s="26" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C239" s="26"/>
       <c r="D239" s="27" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -5867,13 +5878,13 @@
         <v>68</v>
       </c>
       <c r="B240" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="C240" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="C240" s="26" t="s">
+      <c r="D240" s="27" t="s">
         <v>504</v>
-      </c>
-      <c r="D240" s="27" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5881,13 +5892,13 @@
         <v>72</v>
       </c>
       <c r="B241" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="C241" s="26" t="s">
         <v>488</v>
       </c>
-      <c r="C241" s="26" t="s">
+      <c r="D241" s="27" t="s">
         <v>489</v>
-      </c>
-      <c r="D241" s="27" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5895,16 +5906,16 @@
         <v>48</v>
       </c>
       <c r="B242" s="26" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C242" s="26"/>
       <c r="D242" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="5"/>
@@ -5914,13 +5925,13 @@
         <v>1</v>
       </c>
       <c r="B245" s="58" t="s">
+        <v>508</v>
+      </c>
+      <c r="C245" s="58" t="s">
         <v>509</v>
       </c>
-      <c r="C245" s="58" t="s">
+      <c r="D245" s="59" t="s">
         <v>510</v>
-      </c>
-      <c r="D245" s="59" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -5928,13 +5939,13 @@
         <v>22</v>
       </c>
       <c r="B246" s="26" t="s">
+        <v>511</v>
+      </c>
+      <c r="C246" s="26" t="s">
         <v>512</v>
       </c>
-      <c r="C246" s="26" t="s">
+      <c r="D246" s="27" t="s">
         <v>513</v>
-      </c>
-      <c r="D246" s="27" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,13 +5953,13 @@
         <v>5</v>
       </c>
       <c r="B247" s="26" t="s">
+        <v>514</v>
+      </c>
+      <c r="C247" s="26" t="s">
         <v>515</v>
       </c>
-      <c r="C247" s="26" t="s">
+      <c r="D247" s="28" t="s">
         <v>516</v>
-      </c>
-      <c r="D247" s="28" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5956,13 +5967,13 @@
         <v>8</v>
       </c>
       <c r="B248" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="C248" s="26" t="s">
         <v>518</v>
       </c>
-      <c r="C248" s="26" t="s">
+      <c r="D248" s="28" t="s">
         <v>519</v>
-      </c>
-      <c r="D248" s="28" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -5970,13 +5981,13 @@
         <v>11</v>
       </c>
       <c r="B249" s="26" t="s">
+        <v>520</v>
+      </c>
+      <c r="C249" s="26" t="s">
         <v>521</v>
       </c>
-      <c r="C249" s="26" t="s">
+      <c r="D249" s="28" t="s">
         <v>522</v>
-      </c>
-      <c r="D249" s="28" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -5984,13 +5995,13 @@
         <v>14</v>
       </c>
       <c r="B250" s="26" t="s">
+        <v>520</v>
+      </c>
+      <c r="C250" s="26" t="s">
         <v>521</v>
       </c>
-      <c r="C250" s="26" t="s">
+      <c r="D250" s="28" t="s">
         <v>522</v>
-      </c>
-      <c r="D250" s="28" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -5998,18 +6009,18 @@
         <v>68</v>
       </c>
       <c r="B251" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="C251" s="60" t="s">
         <v>524</v>
       </c>
-      <c r="C251" s="60" t="s">
+      <c r="D251" s="28" t="s">
         <v>525</v>
-      </c>
-      <c r="D251" s="28" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="5"/>
@@ -6019,13 +6030,13 @@
         <v>1</v>
       </c>
       <c r="B254" s="26" t="s">
+        <v>527</v>
+      </c>
+      <c r="C254" s="26" t="s">
         <v>528</v>
       </c>
-      <c r="C254" s="26" t="s">
+      <c r="D254" s="27" t="s">
         <v>529</v>
-      </c>
-      <c r="D254" s="27" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -6033,13 +6044,13 @@
         <v>22</v>
       </c>
       <c r="B255" s="26" t="s">
+        <v>530</v>
+      </c>
+      <c r="C255" s="26" t="s">
         <v>531</v>
       </c>
-      <c r="C255" s="26" t="s">
+      <c r="D255" s="27" t="s">
         <v>532</v>
-      </c>
-      <c r="D255" s="27" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -6047,13 +6058,13 @@
         <v>5</v>
       </c>
       <c r="B256" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="C256" s="26" t="s">
         <v>534</v>
       </c>
-      <c r="C256" s="26" t="s">
+      <c r="D256" s="27" t="s">
         <v>535</v>
-      </c>
-      <c r="D256" s="27" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -6061,13 +6072,13 @@
         <v>8</v>
       </c>
       <c r="B257" s="26" t="s">
+        <v>536</v>
+      </c>
+      <c r="C257" s="26" t="s">
         <v>537</v>
       </c>
-      <c r="C257" s="26" t="s">
+      <c r="D257" s="27" t="s">
         <v>538</v>
-      </c>
-      <c r="D257" s="27" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -6075,13 +6086,13 @@
         <v>11</v>
       </c>
       <c r="B258" s="26" t="s">
+        <v>539</v>
+      </c>
+      <c r="C258" s="26" t="s">
         <v>540</v>
       </c>
-      <c r="C258" s="26" t="s">
+      <c r="D258" s="27" t="s">
         <v>541</v>
-      </c>
-      <c r="D258" s="27" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -6089,13 +6100,13 @@
         <v>14</v>
       </c>
       <c r="B259" s="26" t="s">
+        <v>542</v>
+      </c>
+      <c r="C259" s="26" t="s">
         <v>543</v>
       </c>
-      <c r="C259" s="26" t="s">
+      <c r="D259" s="27" t="s">
         <v>544</v>
-      </c>
-      <c r="D259" s="27" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -6103,13 +6114,13 @@
         <v>68</v>
       </c>
       <c r="B260" s="26" t="s">
+        <v>545</v>
+      </c>
+      <c r="C260" s="26" t="s">
         <v>546</v>
       </c>
-      <c r="C260" s="26" t="s">
+      <c r="D260" s="27" t="s">
         <v>547</v>
-      </c>
-      <c r="D260" s="27" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -6117,13 +6128,13 @@
         <v>72</v>
       </c>
       <c r="B261" s="26" t="s">
+        <v>548</v>
+      </c>
+      <c r="C261" s="26" t="s">
         <v>549</v>
       </c>
-      <c r="C261" s="26" t="s">
+      <c r="D261" s="27" t="s">
         <v>550</v>
-      </c>
-      <c r="D261" s="27" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -6131,13 +6142,13 @@
         <v>48</v>
       </c>
       <c r="B262" s="26" t="s">
+        <v>551</v>
+      </c>
+      <c r="C262" s="26" t="s">
         <v>552</v>
       </c>
-      <c r="C262" s="26" t="s">
+      <c r="D262" s="27" t="s">
         <v>553</v>
-      </c>
-      <c r="D262" s="27" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -6145,32 +6156,32 @@
         <v>107</v>
       </c>
       <c r="B263" s="26" t="s">
+        <v>554</v>
+      </c>
+      <c r="C263" s="26" t="s">
         <v>555</v>
       </c>
-      <c r="C263" s="26" t="s">
+      <c r="D263" s="27" t="s">
         <v>556</v>
-      </c>
-      <c r="D263" s="27" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="26" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B264" s="26" t="s">
+        <v>554</v>
+      </c>
+      <c r="C264" s="26" t="s">
         <v>555</v>
       </c>
-      <c r="C264" s="26" t="s">
+      <c r="D264" s="27" t="s">
         <v>556</v>
-      </c>
-      <c r="D264" s="27" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="5"/>
@@ -6180,13 +6191,13 @@
         <v>1</v>
       </c>
       <c r="B267" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="C267" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="C267" s="26" t="s">
+      <c r="D267" s="27" t="s">
         <v>561</v>
-      </c>
-      <c r="D267" s="27" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -6194,13 +6205,13 @@
         <v>22</v>
       </c>
       <c r="B268" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="C268" s="26" t="s">
         <v>563</v>
       </c>
-      <c r="C268" s="26" t="s">
+      <c r="D268" s="27" t="s">
         <v>564</v>
-      </c>
-      <c r="D268" s="27" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -6208,13 +6219,13 @@
         <v>5</v>
       </c>
       <c r="B269" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="C269" s="26" t="s">
         <v>563</v>
       </c>
-      <c r="C269" s="26" t="s">
+      <c r="D269" s="27" t="s">
         <v>564</v>
-      </c>
-      <c r="D269" s="27" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -6222,13 +6233,13 @@
         <v>8</v>
       </c>
       <c r="B270" s="26" t="s">
+        <v>565</v>
+      </c>
+      <c r="C270" s="26" t="s">
         <v>566</v>
       </c>
-      <c r="C270" s="26" t="s">
+      <c r="D270" s="27" t="s">
         <v>567</v>
-      </c>
-      <c r="D270" s="27" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6236,13 +6247,13 @@
         <v>11</v>
       </c>
       <c r="B271" s="26" t="s">
+        <v>568</v>
+      </c>
+      <c r="C271" s="26" t="s">
         <v>569</v>
       </c>
-      <c r="C271" s="26" t="s">
+      <c r="D271" s="27" t="s">
         <v>570</v>
-      </c>
-      <c r="D271" s="27" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -6250,13 +6261,13 @@
         <v>14</v>
       </c>
       <c r="B272" s="26" t="s">
+        <v>568</v>
+      </c>
+      <c r="C272" s="26" t="s">
         <v>569</v>
       </c>
-      <c r="C272" s="26" t="s">
+      <c r="D272" s="27" t="s">
         <v>570</v>
-      </c>
-      <c r="D272" s="27" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -6264,13 +6275,13 @@
         <v>15</v>
       </c>
       <c r="B273" s="26" t="s">
+        <v>568</v>
+      </c>
+      <c r="C273" s="26" t="s">
         <v>569</v>
       </c>
-      <c r="C273" s="26" t="s">
+      <c r="D273" s="27" t="s">
         <v>570</v>
-      </c>
-      <c r="D273" s="27" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6278,13 +6289,13 @@
         <v>72</v>
       </c>
       <c r="B274" s="26" t="s">
+        <v>571</v>
+      </c>
+      <c r="C274" s="26" t="s">
         <v>572</v>
       </c>
-      <c r="C274" s="26" t="s">
+      <c r="D274" s="27" t="s">
         <v>573</v>
-      </c>
-      <c r="D274" s="27" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -6292,18 +6303,18 @@
         <v>48</v>
       </c>
       <c r="B275" s="26" t="s">
+        <v>571</v>
+      </c>
+      <c r="C275" s="26" t="s">
         <v>572</v>
       </c>
-      <c r="C275" s="26" t="s">
+      <c r="D275" s="27" t="s">
         <v>573</v>
-      </c>
-      <c r="D275" s="27" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A277" s="13" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="5"/>
@@ -6313,13 +6324,13 @@
         <v>1</v>
       </c>
       <c r="B278" s="26" t="s">
+        <v>575</v>
+      </c>
+      <c r="C278" s="26" t="s">
         <v>576</v>
       </c>
-      <c r="C278" s="26" t="s">
+      <c r="D278" s="61" t="s">
         <v>577</v>
-      </c>
-      <c r="D278" s="61" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -6327,13 +6338,13 @@
         <v>22</v>
       </c>
       <c r="B279" s="26" t="s">
+        <v>578</v>
+      </c>
+      <c r="C279" s="26" t="s">
         <v>579</v>
       </c>
-      <c r="C279" s="26" t="s">
+      <c r="D279" s="61" t="s">
         <v>580</v>
-      </c>
-      <c r="D279" s="61" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -6341,13 +6352,13 @@
         <v>5</v>
       </c>
       <c r="B280" s="26" t="s">
+        <v>581</v>
+      </c>
+      <c r="C280" s="26" t="s">
         <v>582</v>
       </c>
-      <c r="C280" s="26" t="s">
+      <c r="D280" s="28" t="s">
         <v>583</v>
-      </c>
-      <c r="D280" s="28" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -6355,13 +6366,13 @@
         <v>8</v>
       </c>
       <c r="B281" s="26" t="s">
+        <v>584</v>
+      </c>
+      <c r="C281" s="26" t="s">
         <v>585</v>
       </c>
-      <c r="C281" s="26" t="s">
+      <c r="D281" s="61" t="s">
         <v>586</v>
-      </c>
-      <c r="D281" s="61" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -6369,13 +6380,13 @@
         <v>11</v>
       </c>
       <c r="B282" s="26" t="s">
+        <v>587</v>
+      </c>
+      <c r="C282" s="26" t="s">
         <v>588</v>
       </c>
-      <c r="C282" s="26" t="s">
+      <c r="D282" s="28" t="s">
         <v>589</v>
-      </c>
-      <c r="D282" s="28" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -6383,13 +6394,13 @@
         <v>14</v>
       </c>
       <c r="B283" s="26" t="s">
+        <v>590</v>
+      </c>
+      <c r="C283" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="C283" s="26" t="s">
+      <c r="D283" s="28" t="s">
         <v>592</v>
-      </c>
-      <c r="D283" s="28" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -6405,18 +6416,18 @@
         <v>48</v>
       </c>
       <c r="B285" s="26" t="s">
+        <v>593</v>
+      </c>
+      <c r="C285" s="26" t="s">
         <v>594</v>
       </c>
-      <c r="C285" s="26" t="s">
+      <c r="D285" s="61" t="s">
         <v>595</v>
-      </c>
-      <c r="D285" s="61" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -6426,13 +6437,13 @@
         <v>1</v>
       </c>
       <c r="B288" s="26" t="s">
+        <v>597</v>
+      </c>
+      <c r="C288" s="26" t="s">
         <v>598</v>
       </c>
-      <c r="C288" s="26" t="s">
+      <c r="D288" s="27" t="s">
         <v>599</v>
-      </c>
-      <c r="D288" s="27" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6440,13 +6451,13 @@
         <v>22</v>
       </c>
       <c r="B289" s="26" t="s">
+        <v>600</v>
+      </c>
+      <c r="C289" s="26" t="s">
         <v>601</v>
       </c>
-      <c r="C289" s="26" t="s">
+      <c r="D289" s="27" t="s">
         <v>602</v>
-      </c>
-      <c r="D289" s="27" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6454,13 +6465,13 @@
         <v>5</v>
       </c>
       <c r="B290" s="26" t="s">
+        <v>603</v>
+      </c>
+      <c r="C290" s="26" t="s">
         <v>604</v>
       </c>
-      <c r="C290" s="26" t="s">
+      <c r="D290" s="27" t="s">
         <v>605</v>
-      </c>
-      <c r="D290" s="27" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -6468,13 +6479,13 @@
         <v>8</v>
       </c>
       <c r="B291" s="26" t="s">
+        <v>606</v>
+      </c>
+      <c r="C291" s="26" t="s">
         <v>607</v>
       </c>
-      <c r="C291" s="26" t="s">
+      <c r="D291" s="27" t="s">
         <v>608</v>
-      </c>
-      <c r="D291" s="27" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -6482,13 +6493,13 @@
         <v>11</v>
       </c>
       <c r="B292" s="26" t="s">
+        <v>609</v>
+      </c>
+      <c r="C292" s="26" t="s">
         <v>610</v>
       </c>
-      <c r="C292" s="26" t="s">
+      <c r="D292" s="27" t="s">
         <v>611</v>
-      </c>
-      <c r="D292" s="27" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -6496,27 +6507,27 @@
         <v>14</v>
       </c>
       <c r="B293" s="26" t="s">
+        <v>612</v>
+      </c>
+      <c r="C293" s="26" t="s">
         <v>613</v>
       </c>
-      <c r="C293" s="26" t="s">
+      <c r="D293" s="27" t="s">
         <v>614</v>
-      </c>
-      <c r="D293" s="27" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="26" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B294" s="26" t="s">
+        <v>615</v>
+      </c>
+      <c r="C294" s="26" t="s">
         <v>616</v>
       </c>
-      <c r="C294" s="26" t="s">
+      <c r="D294" s="27" t="s">
         <v>617</v>
-      </c>
-      <c r="D294" s="27" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -6524,7 +6535,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="22" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B296" s="5"/>
       <c r="D296" s="7"/>
@@ -6534,13 +6545,13 @@
         <v>1</v>
       </c>
       <c r="B297" s="26" t="s">
+        <v>619</v>
+      </c>
+      <c r="C297" s="26" t="s">
         <v>620</v>
       </c>
-      <c r="C297" s="26" t="s">
+      <c r="D297" s="26" t="s">
         <v>621</v>
-      </c>
-      <c r="D297" s="26" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -6548,13 +6559,13 @@
         <v>22</v>
       </c>
       <c r="B298" s="26" t="s">
+        <v>622</v>
+      </c>
+      <c r="C298" s="26" t="s">
         <v>623</v>
       </c>
-      <c r="C298" s="26" t="s">
+      <c r="D298" s="26" t="s">
         <v>624</v>
-      </c>
-      <c r="D298" s="26" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -6562,13 +6573,13 @@
         <v>5</v>
       </c>
       <c r="B299" s="26" t="s">
+        <v>625</v>
+      </c>
+      <c r="C299" s="26" t="s">
         <v>626</v>
       </c>
-      <c r="C299" s="26" t="s">
+      <c r="D299" s="26" t="s">
         <v>627</v>
-      </c>
-      <c r="D299" s="26" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -6576,13 +6587,13 @@
         <v>8</v>
       </c>
       <c r="B300" s="26" t="s">
+        <v>628</v>
+      </c>
+      <c r="C300" s="26" t="s">
         <v>629</v>
       </c>
-      <c r="C300" s="26" t="s">
+      <c r="D300" s="26" t="s">
         <v>630</v>
-      </c>
-      <c r="D300" s="26" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -6590,25 +6601,25 @@
         <v>11</v>
       </c>
       <c r="B301" s="26" t="s">
+        <v>631</v>
+      </c>
+      <c r="C301" s="26" t="s">
         <v>632</v>
       </c>
-      <c r="C301" s="26" t="s">
+      <c r="D301" s="26" t="s">
         <v>633</v>
-      </c>
-      <c r="D301" s="26" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="26"/>
       <c r="B302" s="26" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C302" s="26" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D302" s="26" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -6616,7 +6627,7 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A304" s="23" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
@@ -6626,13 +6637,13 @@
         <v>1</v>
       </c>
       <c r="B305" s="26" t="s">
+        <v>636</v>
+      </c>
+      <c r="C305" s="26" t="s">
         <v>637</v>
       </c>
-      <c r="C305" s="26" t="s">
+      <c r="D305" s="27" t="s">
         <v>638</v>
-      </c>
-      <c r="D305" s="27" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -6640,13 +6651,13 @@
         <v>22</v>
       </c>
       <c r="B306" s="26" t="s">
+        <v>639</v>
+      </c>
+      <c r="C306" s="26" t="s">
         <v>640</v>
       </c>
-      <c r="C306" s="26" t="s">
+      <c r="D306" s="27" t="s">
         <v>641</v>
-      </c>
-      <c r="D306" s="27" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -6654,13 +6665,13 @@
         <v>5</v>
       </c>
       <c r="B307" s="26" t="s">
+        <v>642</v>
+      </c>
+      <c r="C307" s="26" t="s">
         <v>643</v>
       </c>
-      <c r="C307" s="26" t="s">
+      <c r="D307" s="27" t="s">
         <v>644</v>
-      </c>
-      <c r="D307" s="27" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -6668,13 +6679,13 @@
         <v>8</v>
       </c>
       <c r="B308" s="26" t="s">
+        <v>645</v>
+      </c>
+      <c r="C308" s="26" t="s">
         <v>646</v>
       </c>
-      <c r="C308" s="26" t="s">
+      <c r="D308" s="27" t="s">
         <v>647</v>
-      </c>
-      <c r="D308" s="27" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -6682,13 +6693,13 @@
         <v>11</v>
       </c>
       <c r="B309" s="26" t="s">
+        <v>648</v>
+      </c>
+      <c r="C309" s="26" t="s">
         <v>649</v>
       </c>
-      <c r="C309" s="26" t="s">
+      <c r="D309" s="27" t="s">
         <v>650</v>
-      </c>
-      <c r="D309" s="27" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -6696,13 +6707,13 @@
         <v>14</v>
       </c>
       <c r="B310" s="26" t="s">
+        <v>651</v>
+      </c>
+      <c r="C310" s="26" t="s">
         <v>652</v>
       </c>
-      <c r="C310" s="26" t="s">
+      <c r="D310" s="27" t="s">
         <v>653</v>
-      </c>
-      <c r="D310" s="27" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -6710,13 +6721,13 @@
         <v>68</v>
       </c>
       <c r="B311" s="26" t="s">
+        <v>654</v>
+      </c>
+      <c r="C311" s="26" t="s">
         <v>655</v>
       </c>
-      <c r="C311" s="26" t="s">
+      <c r="D311" s="27" t="s">
         <v>656</v>
-      </c>
-      <c r="D311" s="27" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -6724,13 +6735,13 @@
         <v>72</v>
       </c>
       <c r="B312" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="C312" s="26" t="s">
         <v>658</v>
       </c>
-      <c r="C312" s="26" t="s">
+      <c r="D312" s="27" t="s">
         <v>659</v>
-      </c>
-      <c r="D312" s="27" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -6738,7 +6749,7 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A314" s="8" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D314" s="21"/>
     </row>
@@ -6747,23 +6758,23 @@
         <v>1</v>
       </c>
       <c r="B315" s="26" t="s">
+        <v>661</v>
+      </c>
+      <c r="C315" s="26" t="s">
         <v>662</v>
       </c>
-      <c r="C315" s="26" t="s">
+      <c r="D315" s="27" t="s">
         <v>663</v>
-      </c>
-      <c r="D315" s="27" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="26"/>
       <c r="B316" s="26" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C316" s="26"/>
       <c r="D316" s="27" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -6771,13 +6782,13 @@
         <v>22</v>
       </c>
       <c r="B317" s="26" t="s">
+        <v>666</v>
+      </c>
+      <c r="C317" s="26" t="s">
         <v>667</v>
       </c>
-      <c r="C317" s="26" t="s">
+      <c r="D317" s="27" t="s">
         <v>668</v>
-      </c>
-      <c r="D317" s="27" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -6785,13 +6796,13 @@
         <v>5</v>
       </c>
       <c r="B318" s="26" t="s">
+        <v>669</v>
+      </c>
+      <c r="C318" s="26" t="s">
         <v>670</v>
       </c>
-      <c r="C318" s="26" t="s">
+      <c r="D318" s="27" t="s">
         <v>671</v>
-      </c>
-      <c r="D318" s="27" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -6799,13 +6810,13 @@
         <v>8</v>
       </c>
       <c r="B319" s="26" t="s">
+        <v>743</v>
+      </c>
+      <c r="C319" s="26" t="s">
         <v>670</v>
       </c>
-      <c r="C319" s="26" t="s">
-        <v>671</v>
-      </c>
-      <c r="D319" s="27" t="s">
-        <v>672</v>
+      <c r="D319" s="61" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -6813,13 +6824,13 @@
         <v>11</v>
       </c>
       <c r="B320" s="26" t="s">
+        <v>672</v>
+      </c>
+      <c r="C320" s="26" t="s">
         <v>673</v>
       </c>
-      <c r="C320" s="26" t="s">
+      <c r="D320" s="27" t="s">
         <v>674</v>
-      </c>
-      <c r="D320" s="27" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -6827,18 +6838,18 @@
         <v>14</v>
       </c>
       <c r="B321" s="26" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C321" s="26" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D321" s="27" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A323" s="13" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="5"/>
@@ -6848,13 +6859,13 @@
         <v>1</v>
       </c>
       <c r="B324" s="26" t="s">
+        <v>677</v>
+      </c>
+      <c r="C324" s="26" t="s">
         <v>678</v>
       </c>
-      <c r="C324" s="26" t="s">
+      <c r="D324" s="27" t="s">
         <v>679</v>
-      </c>
-      <c r="D324" s="27" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -6862,13 +6873,13 @@
         <v>5</v>
       </c>
       <c r="B325" s="26" t="s">
+        <v>680</v>
+      </c>
+      <c r="C325" s="26" t="s">
         <v>681</v>
       </c>
-      <c r="C325" s="26" t="s">
+      <c r="D325" s="27" t="s">
         <v>682</v>
-      </c>
-      <c r="D325" s="27" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -6876,13 +6887,13 @@
         <v>8</v>
       </c>
       <c r="B326" s="26" t="s">
+        <v>683</v>
+      </c>
+      <c r="C326" s="26" t="s">
         <v>684</v>
       </c>
-      <c r="C326" s="26" t="s">
+      <c r="D326" s="27" t="s">
         <v>685</v>
-      </c>
-      <c r="D326" s="27" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -6890,13 +6901,13 @@
         <v>11</v>
       </c>
       <c r="B327" s="26" t="s">
+        <v>686</v>
+      </c>
+      <c r="C327" s="26" t="s">
         <v>687</v>
       </c>
-      <c r="C327" s="26" t="s">
+      <c r="D327" s="27" t="s">
         <v>688</v>
-      </c>
-      <c r="D327" s="27" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6904,13 +6915,13 @@
         <v>14</v>
       </c>
       <c r="B328" s="26" t="s">
+        <v>686</v>
+      </c>
+      <c r="C328" s="26" t="s">
         <v>687</v>
       </c>
-      <c r="C328" s="26" t="s">
+      <c r="D328" s="27" t="s">
         <v>688</v>
-      </c>
-      <c r="D328" s="27" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -6918,13 +6929,13 @@
         <v>68</v>
       </c>
       <c r="B329" s="26" t="s">
+        <v>686</v>
+      </c>
+      <c r="C329" s="26" t="s">
         <v>687</v>
       </c>
-      <c r="C329" s="26" t="s">
+      <c r="D329" s="27" t="s">
         <v>688</v>
-      </c>
-      <c r="D329" s="27" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -6932,18 +6943,18 @@
         <v>72</v>
       </c>
       <c r="B330" s="26" t="s">
+        <v>689</v>
+      </c>
+      <c r="C330" s="26" t="s">
         <v>690</v>
       </c>
-      <c r="C330" s="26" t="s">
+      <c r="D330" s="27" t="s">
         <v>691</v>
-      </c>
-      <c r="D330" s="27" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A332" s="13" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B332" s="24"/>
       <c r="C332" s="25"/>
@@ -6953,13 +6964,13 @@
         <v>1</v>
       </c>
       <c r="B333" s="62" t="s">
+        <v>693</v>
+      </c>
+      <c r="C333" s="62" t="s">
         <v>694</v>
       </c>
-      <c r="C333" s="62" t="s">
+      <c r="D333" s="57" t="s">
         <v>695</v>
-      </c>
-      <c r="D333" s="57" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -6967,13 +6978,13 @@
         <v>22</v>
       </c>
       <c r="B334" s="62" t="s">
+        <v>696</v>
+      </c>
+      <c r="C334" s="62" t="s">
         <v>697</v>
       </c>
-      <c r="C334" s="62" t="s">
+      <c r="D334" s="57" t="s">
         <v>698</v>
-      </c>
-      <c r="D334" s="57" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -6981,13 +6992,13 @@
         <v>5</v>
       </c>
       <c r="B335" s="62" t="s">
+        <v>699</v>
+      </c>
+      <c r="C335" s="62" t="s">
         <v>700</v>
       </c>
-      <c r="C335" s="62" t="s">
+      <c r="D335" s="57" t="s">
         <v>701</v>
-      </c>
-      <c r="D335" s="57" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -6995,13 +7006,13 @@
         <v>8</v>
       </c>
       <c r="B336" s="62" t="s">
+        <v>702</v>
+      </c>
+      <c r="C336" s="62" t="s">
         <v>703</v>
       </c>
-      <c r="C336" s="62" t="s">
+      <c r="D336" s="57" t="s">
         <v>704</v>
-      </c>
-      <c r="D336" s="57" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -7009,13 +7020,13 @@
         <v>11</v>
       </c>
       <c r="B337" s="62" t="s">
+        <v>705</v>
+      </c>
+      <c r="C337" s="62" t="s">
         <v>706</v>
       </c>
-      <c r="C337" s="62" t="s">
+      <c r="D337" s="57" t="s">
         <v>707</v>
-      </c>
-      <c r="D337" s="57" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -7023,13 +7034,13 @@
         <v>14</v>
       </c>
       <c r="B338" s="62" t="s">
+        <v>696</v>
+      </c>
+      <c r="C338" s="62" t="s">
         <v>697</v>
       </c>
-      <c r="C338" s="62" t="s">
+      <c r="D338" s="57" t="s">
         <v>698</v>
-      </c>
-      <c r="D338" s="57" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7037,13 +7048,13 @@
         <v>68</v>
       </c>
       <c r="B339" s="62" t="s">
+        <v>708</v>
+      </c>
+      <c r="C339" s="62" t="s">
         <v>709</v>
       </c>
-      <c r="C339" s="62" t="s">
+      <c r="D339" s="57" t="s">
         <v>710</v>
-      </c>
-      <c r="D339" s="57" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7051,13 +7062,13 @@
         <v>72</v>
       </c>
       <c r="B340" s="62" t="s">
+        <v>711</v>
+      </c>
+      <c r="C340" s="62" t="s">
         <v>712</v>
       </c>
-      <c r="C340" s="62" t="s">
+      <c r="D340" s="57" t="s">
         <v>713</v>
-      </c>
-      <c r="D340" s="57" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7065,41 +7076,41 @@
         <v>48</v>
       </c>
       <c r="B341" s="62" t="s">
+        <v>714</v>
+      </c>
+      <c r="C341" s="62" t="s">
         <v>715</v>
       </c>
-      <c r="C341" s="62" t="s">
+      <c r="D341" s="57" t="s">
         <v>716</v>
-      </c>
-      <c r="D341" s="57" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B342" s="62" t="s">
+        <v>717</v>
+      </c>
+      <c r="C342" s="62" t="s">
         <v>718</v>
       </c>
-      <c r="C342" s="62" t="s">
+      <c r="D342" s="57" t="s">
         <v>719</v>
-      </c>
-      <c r="D342" s="57" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="62" t="s">
+        <v>720</v>
+      </c>
+      <c r="B343" s="62" t="s">
         <v>721</v>
       </c>
-      <c r="B343" s="62" t="s">
+      <c r="C343" s="62" t="s">
         <v>722</v>
       </c>
-      <c r="C343" s="62" t="s">
+      <c r="D343" s="57" t="s">
         <v>723</v>
-      </c>
-      <c r="D343" s="57" t="s">
-        <v>724</v>
       </c>
     </row>
   </sheetData>
@@ -7148,9 +7159,11 @@
     <hyperlink ref="D65" r:id="rId39" display="mailto:darylepare@gmail.com" xr:uid="{FB1E2C3A-4516-44C8-917F-6D55CF54770F}"/>
     <hyperlink ref="D64" r:id="rId40" xr:uid="{52E59539-2E56-4075-90FE-C7622BC19925}"/>
     <hyperlink ref="D66" r:id="rId41" xr:uid="{4ADFA047-8BEA-485C-9922-899E25E27867}"/>
+    <hyperlink ref="D80" r:id="rId42" xr:uid="{9FA6E024-1E52-4D58-AE56-665DF705FF84}"/>
+    <hyperlink ref="D319" r:id="rId43" xr:uid="{9D77423C-C774-4E73-80AC-8111A43E2E15}"/>
   </hyperlinks>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId42"/>
+  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId44"/>
   <rowBreaks count="6" manualBreakCount="6">
     <brk id="47" max="3" man="1"/>
     <brk id="88" max="3" man="1"/>
@@ -7159,6 +7172,6 @@
     <brk id="218" max="3" man="1"/>
     <brk id="264" max="3" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId43"/>
+  <drawing r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SW updated Delta Roster
</commit_message>
<xml_diff>
--- a/secure/club-roster2019.xlsx
+++ b/secure/club-roster2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F0CBC4-28F5-482B-BDE5-443A265656B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A72F51-D1A0-47BF-AD25-9C5DBDE1152F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="690" windowWidth="18225" windowHeight="15510" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
+    <workbookView xWindow="2610" yWindow="1155" windowWidth="20205" windowHeight="14265" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="745">
   <si>
     <t>Beach Grove Golf Club</t>
   </si>
@@ -487,15 +487,6 @@
     <t>darylepare@gmail.com</t>
   </si>
   <si>
-    <t>Carol Mitchell</t>
-  </si>
-  <si>
-    <t>604-951-8223</t>
-  </si>
-  <si>
-    <t>carol_mitchell@telus.net</t>
-  </si>
-  <si>
     <t>Vacant</t>
   </si>
   <si>
@@ -2264,6 +2255,15 @@
   </si>
   <si>
     <t>jmelloywebster@gmail.com</t>
+  </si>
+  <si>
+    <t>Cheri Hallgrimson</t>
+  </si>
+  <si>
+    <t>604-589-9435</t>
+  </si>
+  <si>
+    <t>chetom1@telus.net</t>
   </si>
 </sst>
 </file>
@@ -2273,7 +2273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;###\-###\-####"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2439,6 +2439,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2531,7 +2538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2672,14 +2679,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3104,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EEE842-FA9A-4617-9438-69514D1A7666}">
   <dimension ref="A1:F343"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D343" sqref="A1:D343"/>
+    <sheetView tabSelected="1" topLeftCell="A319" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,10 +3128,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>729</v>
-      </c>
-      <c r="C1" s="65"/>
+      <c r="B1" s="66" t="s">
+        <v>726</v>
+      </c>
+      <c r="C1" s="67"/>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3866,18 +3876,18 @@
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="26"/>
       <c r="B66" s="38" t="s">
-        <v>152</v>
+        <v>742</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D66" s="36" t="s">
-        <v>154</v>
+        <v>743</v>
+      </c>
+      <c r="D66" s="68" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="5"/>
@@ -3887,7 +3897,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C68" s="32"/>
       <c r="D68" s="32"/>
@@ -3897,7 +3907,7 @@
         <v>22</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C69" s="39"/>
       <c r="D69" s="39"/>
@@ -3907,13 +3917,13 @@
         <v>5</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C70" s="39" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3921,13 +3931,13 @@
         <v>8</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C71" s="39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3935,13 +3945,13 @@
         <v>11</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C72" s="39" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,13 +3959,13 @@
         <v>14</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C73" s="39" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3963,13 +3973,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C74" s="39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,13 +3987,13 @@
         <v>48</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D75" s="40" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3993,7 +4003,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="14"/>
@@ -4004,27 +4014,27 @@
         <v>1</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C78" s="39" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="C79" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D79" s="40" t="s">
         <v>179</v>
-      </c>
-      <c r="B79" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="C79" s="39" t="s">
-        <v>181</v>
-      </c>
-      <c r="D79" s="40" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4032,24 +4042,24 @@
         <v>5</v>
       </c>
       <c r="B80" s="39" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C80" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="D80" s="67" t="s">
-        <v>742</v>
+        <v>181</v>
+      </c>
+      <c r="D80" s="65" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
       <c r="D81" s="11"/>
-      <c r="F81" s="66"/>
+      <c r="F81" s="64"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="5"/>
@@ -4059,13 +4069,13 @@
         <v>1</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D83" s="33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -4073,13 +4083,13 @@
         <v>22</v>
       </c>
       <c r="B84" s="32" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D84" s="33" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -4087,13 +4097,13 @@
         <v>5</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C85" s="32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D85" s="33" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -4101,13 +4111,13 @@
         <v>8</v>
       </c>
       <c r="B86" s="32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D86" s="33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -4115,13 +4125,13 @@
         <v>11</v>
       </c>
       <c r="B87" s="32" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -4129,18 +4139,18 @@
         <v>14</v>
       </c>
       <c r="B88" s="32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D88" s="33" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="5"/>
@@ -4150,13 +4160,13 @@
         <v>1</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D91" s="27" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -4164,13 +4174,13 @@
         <v>22</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D92" s="27" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -4178,13 +4188,13 @@
         <v>5</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D93" s="27" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -4192,13 +4202,13 @@
         <v>8</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D94" s="27" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -4206,13 +4216,13 @@
         <v>11</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D95" s="27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -4220,13 +4230,13 @@
         <v>14</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D96" s="27" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4234,13 +4244,13 @@
         <v>72</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D97" s="27" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4248,13 +4258,13 @@
         <v>48</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D98" s="27" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4262,7 +4272,7 @@
     </row>
     <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="5"/>
@@ -4272,13 +4282,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="32" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D101" s="33" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4286,13 +4296,13 @@
         <v>22</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D102" s="33" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4300,13 +4310,13 @@
         <v>5</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D103" s="33" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4314,13 +4324,13 @@
         <v>8</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D104" s="33" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4328,13 +4338,13 @@
         <v>11</v>
       </c>
       <c r="B105" s="32" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D105" s="33" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4342,13 +4352,13 @@
         <v>14</v>
       </c>
       <c r="B106" s="32" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D106" s="33" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4356,13 +4366,13 @@
         <v>72</v>
       </c>
       <c r="B107" s="32" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4370,13 +4380,13 @@
         <v>48</v>
       </c>
       <c r="B108" s="32" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D108" s="33" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,7 +4396,7 @@
     </row>
     <row r="110" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -4397,13 +4407,13 @@
         <v>1</v>
       </c>
       <c r="B111" s="39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C111" s="39" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4411,13 +4421,13 @@
         <v>22</v>
       </c>
       <c r="B112" s="39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C112" s="39" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,13 +4435,13 @@
         <v>5</v>
       </c>
       <c r="B113" s="39" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C113" s="39" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4439,27 +4449,27 @@
         <v>8</v>
       </c>
       <c r="B114" s="39" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C114" s="39" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="B115" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="D115" s="40" t="s">
         <v>261</v>
-      </c>
-      <c r="B115" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="C115" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="D115" s="40" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4467,18 +4477,18 @@
         <v>14</v>
       </c>
       <c r="B116" s="39" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C116" s="39" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D116" s="40" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="5"/>
@@ -4488,13 +4498,13 @@
         <v>1</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C119" s="26" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D119" s="27" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4502,13 +4512,13 @@
         <v>22</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C120" s="26" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D120" s="27" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4516,13 +4526,13 @@
         <v>5</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C121" s="26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D121" s="27" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4530,13 +4540,13 @@
         <v>8</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C122" s="26" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D122" s="27" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4544,13 +4554,13 @@
         <v>11</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C123" s="26" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D123" s="27" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4558,13 +4568,13 @@
         <v>14</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C124" s="26" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D124" s="41" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4572,13 +4582,13 @@
         <v>72</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C125" s="26" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D125" s="27" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4586,13 +4596,13 @@
         <v>48</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C126" s="26" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D126" s="27" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4600,7 +4610,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D128" s="6"/>
     </row>
@@ -4609,13 +4619,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="26" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C129" s="26" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D129" s="26" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4623,13 +4633,13 @@
         <v>22</v>
       </c>
       <c r="B130" s="26" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C130" s="26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D130" s="26" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -4637,7 +4647,7 @@
         <v>5</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C131" s="26"/>
       <c r="D131" s="27"/>
@@ -4647,13 +4657,13 @@
         <v>8</v>
       </c>
       <c r="B132" s="26" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C132" s="26" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D132" s="26" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4661,13 +4671,13 @@
         <v>11</v>
       </c>
       <c r="B133" s="26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C133" s="26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D133" s="26" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4676,7 +4686,7 @@
     </row>
     <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -4684,28 +4694,28 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="26" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B136" s="32" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C136" s="42" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D136" s="33" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="26"/>
       <c r="B137" s="32" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C137" s="43">
         <v>0</v>
       </c>
       <c r="D137" s="33" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4713,10 +4723,10 @@
         <v>8</v>
       </c>
       <c r="B138" s="44" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="C138" s="63" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="D138" s="53">
         <v>0</v>
@@ -4725,7 +4735,7 @@
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="50"/>
       <c r="B139" s="51" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C139" s="52"/>
       <c r="D139" s="54"/>
@@ -4733,7 +4743,7 @@
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="45"/>
       <c r="B140" s="46" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C140" s="47"/>
       <c r="D140" s="48"/>
@@ -4743,11 +4753,11 @@
         <v>8</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C141" s="39"/>
       <c r="D141" s="33" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,11 +4765,11 @@
         <v>11</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C142" s="39"/>
       <c r="D142" s="33" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4767,11 +4777,11 @@
         <v>14</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C143" s="39"/>
       <c r="D143" s="33" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4779,45 +4789,45 @@
         <v>15</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C144" s="26"/>
       <c r="D144" s="33" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="26" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="B145" s="32"/>
       <c r="C145" s="26"/>
       <c r="D145" s="33" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="31" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C146" s="26"/>
       <c r="D146" s="33" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="26" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C147" s="26"/>
       <c r="D147" s="33" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4826,7 +4836,7 @@
     </row>
     <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D149" s="7"/>
     </row>
@@ -4835,13 +4845,13 @@
         <v>1</v>
       </c>
       <c r="B150" s="26" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C150" s="26" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D150" s="27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4850,7 +4860,7 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="5"/>
@@ -4860,13 +4870,13 @@
         <v>1</v>
       </c>
       <c r="B153" s="32" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C153" s="32" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D153" s="33" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4874,13 +4884,13 @@
         <v>22</v>
       </c>
       <c r="B154" s="39" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C154" s="39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D154" s="40" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4888,13 +4898,13 @@
         <v>5</v>
       </c>
       <c r="B155" s="39" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C155" s="39" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D155" s="40" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4902,13 +4912,13 @@
         <v>8</v>
       </c>
       <c r="B156" s="39" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C156" s="39" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D156" s="40" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4916,13 +4926,13 @@
         <v>11</v>
       </c>
       <c r="B157" s="39" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C157" s="39" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D157" s="40" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4930,13 +4940,13 @@
         <v>14</v>
       </c>
       <c r="B158" s="39" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C158" s="39" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D158" s="40" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4944,25 +4954,25 @@
         <v>72</v>
       </c>
       <c r="B159" s="39" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C159" s="39" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D159" s="40" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="26"/>
       <c r="B160" s="39" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C160" s="39" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D160" s="40" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4970,13 +4980,13 @@
         <v>48</v>
       </c>
       <c r="B161" s="39" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C161" s="39" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D161" s="40" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4996,7 @@
     </row>
     <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="14"/>
@@ -4997,27 +5007,27 @@
         <v>1</v>
       </c>
       <c r="B164" s="39" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C164" s="39" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D164" s="40" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="26" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B165" s="39" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C165" s="39" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D165" s="40" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5025,13 +5035,13 @@
         <v>5</v>
       </c>
       <c r="B166" s="39" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C166" s="39" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D166" s="40" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -5041,7 +5051,7 @@
     </row>
     <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="5"/>
@@ -5051,13 +5061,13 @@
         <v>1</v>
       </c>
       <c r="B169" s="32" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C169" s="32" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D169" s="55" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -5065,13 +5075,13 @@
         <v>22</v>
       </c>
       <c r="B170" s="39" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C170" s="39" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D170" s="56" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5079,11 +5089,11 @@
         <v>5</v>
       </c>
       <c r="B171" s="39" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C171" s="39"/>
       <c r="D171" s="56" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,13 +5101,13 @@
         <v>8</v>
       </c>
       <c r="B172" s="39" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C172" s="39" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D172" s="56" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,13 +5115,13 @@
         <v>11</v>
       </c>
       <c r="B173" s="39" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C173" s="39" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D173" s="56" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5119,13 +5129,13 @@
         <v>14</v>
       </c>
       <c r="B174" s="39" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C174" s="39" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D174" s="56" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -5133,13 +5143,13 @@
         <v>48</v>
       </c>
       <c r="B175" s="39" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C175" s="39" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D175" s="36" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -5149,7 +5159,7 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B177" s="2"/>
       <c r="D177" s="7"/>
@@ -5159,13 +5169,13 @@
         <v>1</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C178" s="26" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D178" s="27" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -5173,13 +5183,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C179" s="26" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D179" s="27" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -5187,13 +5197,13 @@
         <v>5</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C180" s="26" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D180" s="27" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -5201,13 +5211,13 @@
         <v>8</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C181" s="26" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D181" s="27" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -5215,13 +5225,13 @@
         <v>11</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C182" s="26" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D182" s="27" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -5229,13 +5239,13 @@
         <v>14</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C183" s="26" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D183" s="28" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5245,7 +5255,7 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="5"/>
@@ -5255,27 +5265,27 @@
         <v>1</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C186" s="26" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D186" s="27" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="B187" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="C187" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="D187" s="27" t="s">
         <v>397</v>
-      </c>
-      <c r="B187" s="26" t="s">
-        <v>398</v>
-      </c>
-      <c r="C187" s="26" t="s">
-        <v>399</v>
-      </c>
-      <c r="D187" s="27" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5283,13 +5293,13 @@
         <v>5</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C188" s="26" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D188" s="27" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5297,13 +5307,13 @@
         <v>8</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C189" s="26" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D189" s="27" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5311,13 +5321,13 @@
         <v>11</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C190" s="26" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D190" s="27" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5325,13 +5335,13 @@
         <v>14</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C191" s="26" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D191" s="27" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5339,18 +5349,18 @@
         <v>48</v>
       </c>
       <c r="B192" s="26" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C192" s="26" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D192" s="27" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="5"/>
@@ -5360,13 +5370,13 @@
         <v>1</v>
       </c>
       <c r="B195" s="26" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C195" s="26" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D195" s="27" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5374,13 +5384,13 @@
         <v>22</v>
       </c>
       <c r="B196" s="26" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D196" s="27" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5388,13 +5398,13 @@
         <v>5</v>
       </c>
       <c r="B197" s="26" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C197" s="26" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D197" s="27" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5402,13 +5412,13 @@
         <v>8</v>
       </c>
       <c r="B198" s="26" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C198" s="26" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D198" s="27" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5416,18 +5426,18 @@
         <v>14</v>
       </c>
       <c r="B199" s="26" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C199" s="26" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D199" s="27" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
@@ -5437,13 +5447,13 @@
         <v>1</v>
       </c>
       <c r="B202" s="26" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C202" s="26" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D202" s="27" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5451,13 +5461,13 @@
         <v>22</v>
       </c>
       <c r="B203" s="26" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C203" s="26" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D203" s="27" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5465,13 +5475,13 @@
         <v>5</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C204" s="26" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D204" s="27" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5479,13 +5489,13 @@
         <v>8</v>
       </c>
       <c r="B205" s="26" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C205" s="26" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D205" s="27" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5493,13 +5503,13 @@
         <v>11</v>
       </c>
       <c r="B206" s="26" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C206" s="26" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D206" s="27" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,13 +5517,13 @@
         <v>14</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C207" s="26" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D207" s="27" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5521,7 +5531,7 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D209" s="7"/>
     </row>
@@ -5530,13 +5540,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="26" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C210" s="26" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D210" s="27" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5544,13 +5554,13 @@
         <v>22</v>
       </c>
       <c r="B211" s="26" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C211" s="26" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D211" s="27" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5558,11 +5568,11 @@
         <v>5</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C212" s="26"/>
       <c r="D212" s="27" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5578,11 +5588,11 @@
         <v>14</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C214" s="26"/>
       <c r="D214" s="27" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5590,11 +5600,11 @@
         <v>15</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C215" s="26"/>
       <c r="D215" s="27" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5602,13 +5612,13 @@
         <v>68</v>
       </c>
       <c r="B216" s="26" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C216" s="26" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D216" s="27" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5616,13 +5626,13 @@
         <v>72</v>
       </c>
       <c r="B217" s="26" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C217" s="26" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D217" s="27" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5630,13 +5640,13 @@
         <v>48</v>
       </c>
       <c r="B218" s="26" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C218" s="26" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D218" s="27" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5645,7 +5655,7 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D220" s="7"/>
     </row>
@@ -5654,13 +5664,13 @@
         <v>1</v>
       </c>
       <c r="B221" s="26" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C221" s="26" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D221" s="27" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5668,13 +5678,13 @@
         <v>22</v>
       </c>
       <c r="B222" s="26" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C222" s="26" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D222" s="27" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5682,13 +5692,13 @@
         <v>5</v>
       </c>
       <c r="B223" s="26" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C223" s="26" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D223" s="27" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5696,13 +5706,13 @@
         <v>8</v>
       </c>
       <c r="B224" s="26" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C224" s="26" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D224" s="27" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5710,13 +5720,13 @@
         <v>11</v>
       </c>
       <c r="B225" s="26" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C225" s="26" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D225" s="27" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5724,13 +5734,13 @@
         <v>14</v>
       </c>
       <c r="B226" s="26" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C226" s="26" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D226" s="27" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5738,13 +5748,13 @@
         <v>68</v>
       </c>
       <c r="B227" s="26" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C227" s="26" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D227" s="27" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5768,13 +5778,13 @@
         <v>107</v>
       </c>
       <c r="B230" s="26" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C230" s="26" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D230" s="57" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5782,7 +5792,7 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B232" s="4"/>
       <c r="C232" s="5"/>
@@ -5792,13 +5802,13 @@
         <v>1</v>
       </c>
       <c r="B233" s="26" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C233" s="26" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D233" s="27" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5806,13 +5816,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="26" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C234" s="26" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D234" s="27" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5820,13 +5830,13 @@
         <v>5</v>
       </c>
       <c r="B235" s="26" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C235" s="26" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D235" s="27" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5834,11 +5844,11 @@
         <v>8</v>
       </c>
       <c r="B236" s="26" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C236" s="26"/>
       <c r="D236" s="27" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5854,11 +5864,11 @@
         <v>14</v>
       </c>
       <c r="B238" s="26" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C238" s="26"/>
       <c r="D238" s="27" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -5866,11 +5876,11 @@
         <v>15</v>
       </c>
       <c r="B239" s="26" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C239" s="26"/>
       <c r="D239" s="27" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -5878,13 +5888,13 @@
         <v>68</v>
       </c>
       <c r="B240" s="26" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C240" s="26" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D240" s="27" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5892,13 +5902,13 @@
         <v>72</v>
       </c>
       <c r="B241" s="26" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C241" s="26" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D241" s="27" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5906,16 +5916,16 @@
         <v>48</v>
       </c>
       <c r="B242" s="26" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C242" s="26"/>
       <c r="D242" s="27" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="5"/>
@@ -5925,13 +5935,13 @@
         <v>1</v>
       </c>
       <c r="B245" s="58" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C245" s="58" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D245" s="59" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -5939,13 +5949,13 @@
         <v>22</v>
       </c>
       <c r="B246" s="26" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C246" s="26" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D246" s="27" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -5953,13 +5963,13 @@
         <v>5</v>
       </c>
       <c r="B247" s="26" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C247" s="26" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D247" s="28" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5967,13 +5977,13 @@
         <v>8</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C248" s="26" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D248" s="28" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -5981,13 +5991,13 @@
         <v>11</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C249" s="26" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D249" s="28" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -5995,13 +6005,13 @@
         <v>14</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C250" s="26" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D250" s="28" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -6009,18 +6019,18 @@
         <v>68</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C251" s="60" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D251" s="28" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="5"/>
@@ -6030,13 +6040,13 @@
         <v>1</v>
       </c>
       <c r="B254" s="26" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C254" s="26" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D254" s="27" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -6044,13 +6054,13 @@
         <v>22</v>
       </c>
       <c r="B255" s="26" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C255" s="26" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D255" s="27" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -6058,13 +6068,13 @@
         <v>5</v>
       </c>
       <c r="B256" s="26" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C256" s="26" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D256" s="27" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -6072,13 +6082,13 @@
         <v>8</v>
       </c>
       <c r="B257" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C257" s="26" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D257" s="27" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -6086,13 +6096,13 @@
         <v>11</v>
       </c>
       <c r="B258" s="26" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C258" s="26" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D258" s="27" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -6100,13 +6110,13 @@
         <v>14</v>
       </c>
       <c r="B259" s="26" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C259" s="26" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D259" s="27" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -6114,13 +6124,13 @@
         <v>68</v>
       </c>
       <c r="B260" s="26" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C260" s="26" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D260" s="27" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -6128,13 +6138,13 @@
         <v>72</v>
       </c>
       <c r="B261" s="26" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C261" s="26" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D261" s="27" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -6142,13 +6152,13 @@
         <v>48</v>
       </c>
       <c r="B262" s="26" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C262" s="26" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D262" s="27" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -6156,32 +6166,32 @@
         <v>107</v>
       </c>
       <c r="B263" s="26" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C263" s="26" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D263" s="27" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="26" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B264" s="26" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C264" s="26" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D264" s="27" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="5"/>
@@ -6191,13 +6201,13 @@
         <v>1</v>
       </c>
       <c r="B267" s="26" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C267" s="26" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D267" s="27" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -6205,13 +6215,13 @@
         <v>22</v>
       </c>
       <c r="B268" s="26" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C268" s="26" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D268" s="27" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -6219,13 +6229,13 @@
         <v>5</v>
       </c>
       <c r="B269" s="26" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C269" s="26" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D269" s="27" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -6233,13 +6243,13 @@
         <v>8</v>
       </c>
       <c r="B270" s="26" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C270" s="26" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D270" s="27" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6247,13 +6257,13 @@
         <v>11</v>
       </c>
       <c r="B271" s="26" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C271" s="26" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D271" s="27" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -6261,13 +6271,13 @@
         <v>14</v>
       </c>
       <c r="B272" s="26" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C272" s="26" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D272" s="27" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -6275,13 +6285,13 @@
         <v>15</v>
       </c>
       <c r="B273" s="26" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C273" s="26" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D273" s="27" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6289,13 +6299,13 @@
         <v>72</v>
       </c>
       <c r="B274" s="26" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C274" s="26" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D274" s="27" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -6303,18 +6313,18 @@
         <v>48</v>
       </c>
       <c r="B275" s="26" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C275" s="26" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D275" s="27" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A277" s="13" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="5"/>
@@ -6324,13 +6334,13 @@
         <v>1</v>
       </c>
       <c r="B278" s="26" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C278" s="26" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D278" s="61" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -6338,13 +6348,13 @@
         <v>22</v>
       </c>
       <c r="B279" s="26" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C279" s="26" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D279" s="61" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -6352,13 +6362,13 @@
         <v>5</v>
       </c>
       <c r="B280" s="26" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C280" s="26" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D280" s="28" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -6366,13 +6376,13 @@
         <v>8</v>
       </c>
       <c r="B281" s="26" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C281" s="26" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D281" s="61" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -6380,13 +6390,13 @@
         <v>11</v>
       </c>
       <c r="B282" s="26" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C282" s="26" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D282" s="28" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -6394,13 +6404,13 @@
         <v>14</v>
       </c>
       <c r="B283" s="26" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C283" s="26" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D283" s="28" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -6416,18 +6426,18 @@
         <v>48</v>
       </c>
       <c r="B285" s="26" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C285" s="26" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D285" s="61" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -6437,13 +6447,13 @@
         <v>1</v>
       </c>
       <c r="B288" s="26" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C288" s="26" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D288" s="27" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6451,13 +6461,13 @@
         <v>22</v>
       </c>
       <c r="B289" s="26" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C289" s="26" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D289" s="27" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6465,13 +6475,13 @@
         <v>5</v>
       </c>
       <c r="B290" s="26" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C290" s="26" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D290" s="27" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -6479,13 +6489,13 @@
         <v>8</v>
       </c>
       <c r="B291" s="26" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C291" s="26" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D291" s="27" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -6493,13 +6503,13 @@
         <v>11</v>
       </c>
       <c r="B292" s="26" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C292" s="26" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D292" s="27" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -6507,27 +6517,27 @@
         <v>14</v>
       </c>
       <c r="B293" s="26" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C293" s="26" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D293" s="27" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="26" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B294" s="26" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C294" s="26" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D294" s="27" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -6535,7 +6545,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="22" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="B296" s="5"/>
       <c r="D296" s="7"/>
@@ -6545,13 +6555,13 @@
         <v>1</v>
       </c>
       <c r="B297" s="26" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C297" s="26" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D297" s="26" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -6559,13 +6569,13 @@
         <v>22</v>
       </c>
       <c r="B298" s="26" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C298" s="26" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D298" s="26" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -6573,13 +6583,13 @@
         <v>5</v>
       </c>
       <c r="B299" s="26" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C299" s="26" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D299" s="26" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -6587,13 +6597,13 @@
         <v>8</v>
       </c>
       <c r="B300" s="26" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C300" s="26" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D300" s="26" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -6601,25 +6611,25 @@
         <v>11</v>
       </c>
       <c r="B301" s="26" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C301" s="26" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D301" s="26" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="26"/>
       <c r="B302" s="26" t="s">
+        <v>628</v>
+      </c>
+      <c r="C302" s="26" t="s">
         <v>631</v>
       </c>
-      <c r="C302" s="26" t="s">
-        <v>634</v>
-      </c>
       <c r="D302" s="26" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -6627,7 +6637,7 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A304" s="23" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
@@ -6637,13 +6647,13 @@
         <v>1</v>
       </c>
       <c r="B305" s="26" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C305" s="26" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D305" s="27" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -6651,13 +6661,13 @@
         <v>22</v>
       </c>
       <c r="B306" s="26" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C306" s="26" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D306" s="27" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -6665,13 +6675,13 @@
         <v>5</v>
       </c>
       <c r="B307" s="26" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C307" s="26" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D307" s="27" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -6679,13 +6689,13 @@
         <v>8</v>
       </c>
       <c r="B308" s="26" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C308" s="26" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D308" s="27" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -6693,13 +6703,13 @@
         <v>11</v>
       </c>
       <c r="B309" s="26" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C309" s="26" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D309" s="27" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -6707,13 +6717,13 @@
         <v>14</v>
       </c>
       <c r="B310" s="26" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C310" s="26" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="D310" s="27" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -6721,13 +6731,13 @@
         <v>68</v>
       </c>
       <c r="B311" s="26" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="C311" s="26" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D311" s="27" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -6735,13 +6745,13 @@
         <v>72</v>
       </c>
       <c r="B312" s="26" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C312" s="26" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D312" s="27" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -6749,7 +6759,7 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A314" s="8" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D314" s="21"/>
     </row>
@@ -6758,23 +6768,23 @@
         <v>1</v>
       </c>
       <c r="B315" s="26" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C315" s="26" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D315" s="27" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="26"/>
       <c r="B316" s="26" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C316" s="26"/>
       <c r="D316" s="27" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -6782,13 +6792,13 @@
         <v>22</v>
       </c>
       <c r="B317" s="26" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C317" s="26" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D317" s="27" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -6796,13 +6806,13 @@
         <v>5</v>
       </c>
       <c r="B318" s="26" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C318" s="26" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D318" s="27" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -6810,13 +6820,13 @@
         <v>8</v>
       </c>
       <c r="B319" s="26" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C319" s="26" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D319" s="61" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -6824,13 +6834,13 @@
         <v>11</v>
       </c>
       <c r="B320" s="26" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C320" s="26" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D320" s="27" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -6838,18 +6848,18 @@
         <v>14</v>
       </c>
       <c r="B321" s="26" t="s">
+        <v>669</v>
+      </c>
+      <c r="C321" s="26" t="s">
         <v>672</v>
       </c>
-      <c r="C321" s="26" t="s">
-        <v>675</v>
-      </c>
       <c r="D321" s="27" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A323" s="13" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="5"/>
@@ -6859,13 +6869,13 @@
         <v>1</v>
       </c>
       <c r="B324" s="26" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C324" s="26" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D324" s="27" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -6873,13 +6883,13 @@
         <v>5</v>
       </c>
       <c r="B325" s="26" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="C325" s="26" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D325" s="27" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -6887,13 +6897,13 @@
         <v>8</v>
       </c>
       <c r="B326" s="26" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="C326" s="26" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D326" s="27" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -6901,13 +6911,13 @@
         <v>11</v>
       </c>
       <c r="B327" s="26" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C327" s="26" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D327" s="27" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6915,13 +6925,13 @@
         <v>14</v>
       </c>
       <c r="B328" s="26" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C328" s="26" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D328" s="27" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -6929,13 +6939,13 @@
         <v>68</v>
       </c>
       <c r="B329" s="26" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="C329" s="26" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D329" s="27" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -6943,18 +6953,18 @@
         <v>72</v>
       </c>
       <c r="B330" s="26" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C330" s="26" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D330" s="27" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A332" s="13" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="B332" s="24"/>
       <c r="C332" s="25"/>
@@ -6964,13 +6974,13 @@
         <v>1</v>
       </c>
       <c r="B333" s="62" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C333" s="62" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D333" s="57" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -6978,13 +6988,13 @@
         <v>22</v>
       </c>
       <c r="B334" s="62" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C334" s="62" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D334" s="57" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -6992,13 +7002,13 @@
         <v>5</v>
       </c>
       <c r="B335" s="62" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="C335" s="62" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D335" s="57" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -7006,13 +7016,13 @@
         <v>8</v>
       </c>
       <c r="B336" s="62" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="C336" s="62" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D336" s="57" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -7020,13 +7030,13 @@
         <v>11</v>
       </c>
       <c r="B337" s="62" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C337" s="62" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D337" s="57" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -7034,13 +7044,13 @@
         <v>14</v>
       </c>
       <c r="B338" s="62" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C338" s="62" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D338" s="57" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7048,13 +7058,13 @@
         <v>68</v>
       </c>
       <c r="B339" s="62" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="C339" s="62" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="D339" s="57" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7062,13 +7072,13 @@
         <v>72</v>
       </c>
       <c r="B340" s="62" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="C340" s="62" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="D340" s="57" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7076,41 +7086,41 @@
         <v>48</v>
       </c>
       <c r="B341" s="62" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="C341" s="62" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D341" s="57" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="62" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B342" s="62" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="C342" s="62" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D342" s="57" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="62" t="s">
+        <v>717</v>
+      </c>
+      <c r="B343" s="62" t="s">
+        <v>718</v>
+      </c>
+      <c r="C343" s="62" t="s">
+        <v>719</v>
+      </c>
+      <c r="D343" s="57" t="s">
         <v>720</v>
-      </c>
-      <c r="B343" s="62" t="s">
-        <v>721</v>
-      </c>
-      <c r="C343" s="62" t="s">
-        <v>722</v>
-      </c>
-      <c r="D343" s="57" t="s">
-        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SW modified Team Captain info
</commit_message>
<xml_diff>
--- a/secure/club-roster2019.xlsx
+++ b/secure/club-roster2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A72F51-D1A0-47BF-AD25-9C5DBDE1152F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C12613-F7F8-4626-BCB9-D7869E598978}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="1155" windowWidth="20205" windowHeight="14265" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
+    <workbookView xWindow="1470" yWindow="540" windowWidth="22050" windowHeight="14265" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="745">
   <si>
     <t>Beach Grove Golf Club</t>
   </si>
@@ -265,9 +265,6 @@
     <t>604-544-4231</t>
   </si>
   <si>
-    <t>maclogan@shaw.ca</t>
-  </si>
-  <si>
     <t>Capilano Golf &amp; Country Club</t>
   </si>
   <si>
@@ -2264,6 +2261,9 @@
   </si>
   <si>
     <t>chetom1@telus.net</t>
+  </si>
+  <si>
+    <t>macclogan@shaw.ca</t>
   </si>
 </sst>
 </file>
@@ -2683,14 +2683,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3114,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EEE842-FA9A-4617-9438-69514D1A7666}">
   <dimension ref="A1:F343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D343"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3128,10 +3128,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="66" t="s">
-        <v>726</v>
-      </c>
-      <c r="C1" s="67"/>
+      <c r="B1" s="67" t="s">
+        <v>725</v>
+      </c>
+      <c r="C1" s="68"/>
       <c r="D1"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3506,13 +3506,13 @@
       <c r="C34" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="30" t="s">
-        <v>78</v>
+      <c r="D34" s="65" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="5"/>
     </row>
@@ -3521,13 +3521,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="32" t="s">
+      <c r="D37" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="D37" s="33" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3535,13 +3535,13 @@
         <v>22</v>
       </c>
       <c r="B38" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="D38" s="34" t="s">
         <v>84</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3555,13 +3555,13 @@
         <v>5</v>
       </c>
       <c r="B40" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="D40" s="35" t="s">
         <v>87</v>
-      </c>
-      <c r="D40" s="35" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3569,13 +3569,13 @@
         <v>8</v>
       </c>
       <c r="B41" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="32" t="s">
+      <c r="D41" s="34" t="s">
         <v>90</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3583,13 +3583,13 @@
         <v>11</v>
       </c>
       <c r="B42" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="32" t="s">
+      <c r="D42" s="35" t="s">
         <v>93</v>
-      </c>
-      <c r="D42" s="35" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3597,13 +3597,13 @@
         <v>14</v>
       </c>
       <c r="B43" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="D43" s="34" t="s">
         <v>96</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3611,13 +3611,13 @@
         <v>15</v>
       </c>
       <c r="B44" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="D44" s="35" t="s">
         <v>99</v>
-      </c>
-      <c r="D44" s="35" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,39 +3625,39 @@
         <v>68</v>
       </c>
       <c r="B45" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="D45" s="35" t="s">
         <v>102</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
       <c r="B46" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="32" t="s">
+      <c r="D46" s="35" t="s">
         <v>105</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="C47" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="D47" s="27" t="s">
         <v>109</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,7 +3665,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -3675,13 +3675,13 @@
         <v>1</v>
       </c>
       <c r="B50" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="D50" s="28" t="s">
         <v>113</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3689,13 +3689,13 @@
         <v>22</v>
       </c>
       <c r="B51" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="D51" s="36" t="s">
         <v>116</v>
-      </c>
-      <c r="D51" s="36" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3703,13 +3703,13 @@
         <v>5</v>
       </c>
       <c r="B52" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="D52" s="36" t="s">
         <v>119</v>
-      </c>
-      <c r="D52" s="36" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,13 +3717,13 @@
         <v>8</v>
       </c>
       <c r="B53" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="D53" s="36" t="s">
         <v>122</v>
-      </c>
-      <c r="D53" s="36" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3731,13 +3731,13 @@
         <v>11</v>
       </c>
       <c r="B54" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="D54" s="36" t="s">
         <v>125</v>
-      </c>
-      <c r="D54" s="36" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3745,13 +3745,13 @@
         <v>14</v>
       </c>
       <c r="B55" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="D55" s="36" t="s">
         <v>128</v>
-      </c>
-      <c r="D55" s="36" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3759,18 +3759,18 @@
         <v>48</v>
       </c>
       <c r="B56" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="29" t="s">
+      <c r="D56" s="36" t="s">
         <v>125</v>
-      </c>
-      <c r="D56" s="36" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="5"/>
@@ -3780,13 +3780,13 @@
         <v>1</v>
       </c>
       <c r="B59" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="D59" s="28" t="s">
         <v>132</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3794,13 +3794,13 @@
         <v>22</v>
       </c>
       <c r="B60" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C60" s="38" t="s">
+      <c r="D60" s="36" t="s">
         <v>135</v>
-      </c>
-      <c r="D60" s="36" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3808,13 +3808,13 @@
         <v>5</v>
       </c>
       <c r="B61" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="D61" s="28" t="s">
         <v>138</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3822,13 +3822,13 @@
         <v>8</v>
       </c>
       <c r="B62" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="D62" s="28" t="s">
         <v>141</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3836,13 +3836,13 @@
         <v>11</v>
       </c>
       <c r="B63" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="C63" s="26" t="s">
+      <c r="D63" s="28" t="s">
         <v>144</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3850,13 +3850,13 @@
         <v>14</v>
       </c>
       <c r="B64" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C64" s="38" t="s">
+      <c r="D64" s="36" t="s">
         <v>147</v>
-      </c>
-      <c r="D64" s="36" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3864,30 +3864,30 @@
         <v>48</v>
       </c>
       <c r="B65" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C65" s="38" t="s">
+      <c r="D65" s="36" t="s">
         <v>150</v>
-      </c>
-      <c r="D65" s="36" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="26"/>
       <c r="B66" s="38" t="s">
+        <v>741</v>
+      </c>
+      <c r="C66" s="38" t="s">
         <v>742</v>
       </c>
-      <c r="C66" s="38" t="s">
+      <c r="D66" s="66" t="s">
         <v>743</v>
-      </c>
-      <c r="D66" s="68" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="5"/>
@@ -3897,7 +3897,7 @@
         <v>1</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C68" s="32"/>
       <c r="D68" s="32"/>
@@ -3907,7 +3907,7 @@
         <v>22</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C69" s="39"/>
       <c r="D69" s="39"/>
@@ -3917,13 +3917,13 @@
         <v>5</v>
       </c>
       <c r="B70" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C70" s="39" t="s">
+      <c r="D70" s="40" t="s">
         <v>155</v>
-      </c>
-      <c r="D70" s="40" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3931,13 +3931,13 @@
         <v>8</v>
       </c>
       <c r="B71" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C71" s="39" t="s">
+      <c r="D71" s="40" t="s">
         <v>158</v>
-      </c>
-      <c r="D71" s="40" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3945,13 +3945,13 @@
         <v>11</v>
       </c>
       <c r="B72" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="C72" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="D72" s="40" t="s">
         <v>161</v>
-      </c>
-      <c r="D72" s="40" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3959,13 +3959,13 @@
         <v>14</v>
       </c>
       <c r="B73" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="C73" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="39" t="s">
+      <c r="D73" s="40" t="s">
         <v>164</v>
-      </c>
-      <c r="D73" s="40" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3973,13 +3973,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="C74" s="39" t="s">
+      <c r="D74" s="40" t="s">
         <v>167</v>
-      </c>
-      <c r="D74" s="40" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3987,13 +3987,13 @@
         <v>48</v>
       </c>
       <c r="B75" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="C75" s="39" t="s">
+      <c r="D75" s="40" t="s">
         <v>170</v>
-      </c>
-      <c r="D75" s="40" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4003,7 +4003,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="14"/>
@@ -4014,27 +4014,27 @@
         <v>1</v>
       </c>
       <c r="B78" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C78" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="C78" s="39" t="s">
+      <c r="D78" s="40" t="s">
         <v>174</v>
-      </c>
-      <c r="D78" s="40" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B79" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="B79" s="39" t="s">
+      <c r="C79" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="C79" s="39" t="s">
+      <c r="D79" s="40" t="s">
         <v>178</v>
-      </c>
-      <c r="D79" s="40" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4042,13 +4042,13 @@
         <v>5</v>
       </c>
       <c r="B80" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="C80" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="C80" s="39" t="s">
-        <v>181</v>
-      </c>
       <c r="D80" s="65" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -4059,7 +4059,7 @@
     </row>
     <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="5"/>
@@ -4069,13 +4069,13 @@
         <v>1</v>
       </c>
       <c r="B83" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="C83" s="32" t="s">
+      <c r="D83" s="33" t="s">
         <v>184</v>
-      </c>
-      <c r="D83" s="33" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -4083,13 +4083,13 @@
         <v>22</v>
       </c>
       <c r="B84" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="C84" s="32" t="s">
+      <c r="D84" s="33" t="s">
         <v>187</v>
-      </c>
-      <c r="D84" s="33" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -4097,13 +4097,13 @@
         <v>5</v>
       </c>
       <c r="B85" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C85" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="C85" s="32" t="s">
+      <c r="D85" s="33" t="s">
         <v>190</v>
-      </c>
-      <c r="D85" s="33" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -4111,13 +4111,13 @@
         <v>8</v>
       </c>
       <c r="B86" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C86" s="32" t="s">
+      <c r="D86" s="33" t="s">
         <v>193</v>
-      </c>
-      <c r="D86" s="33" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -4125,13 +4125,13 @@
         <v>11</v>
       </c>
       <c r="B87" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="C87" s="32" t="s">
+      <c r="D87" s="33" t="s">
         <v>196</v>
-      </c>
-      <c r="D87" s="33" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -4139,18 +4139,18 @@
         <v>14</v>
       </c>
       <c r="B88" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="32" t="s">
+      <c r="D88" s="33" t="s">
         <v>199</v>
-      </c>
-      <c r="D88" s="33" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="5"/>
@@ -4160,13 +4160,13 @@
         <v>1</v>
       </c>
       <c r="B91" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C91" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="D91" s="27" t="s">
         <v>203</v>
-      </c>
-      <c r="D91" s="27" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -4174,13 +4174,13 @@
         <v>22</v>
       </c>
       <c r="B92" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C92" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="C92" s="26" t="s">
+      <c r="D92" s="27" t="s">
         <v>206</v>
-      </c>
-      <c r="D92" s="27" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -4188,13 +4188,13 @@
         <v>5</v>
       </c>
       <c r="B93" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C93" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C93" s="26" t="s">
+      <c r="D93" s="27" t="s">
         <v>209</v>
-      </c>
-      <c r="D93" s="27" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -4202,13 +4202,13 @@
         <v>8</v>
       </c>
       <c r="B94" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="C94" s="26" t="s">
+      <c r="D94" s="27" t="s">
         <v>212</v>
-      </c>
-      <c r="D94" s="27" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -4216,13 +4216,13 @@
         <v>11</v>
       </c>
       <c r="B95" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="C95" s="26" t="s">
+      <c r="D95" s="27" t="s">
         <v>215</v>
-      </c>
-      <c r="D95" s="27" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -4230,13 +4230,13 @@
         <v>14</v>
       </c>
       <c r="B96" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="C96" s="26" t="s">
+      <c r="D96" s="27" t="s">
         <v>218</v>
-      </c>
-      <c r="D96" s="27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4244,13 +4244,13 @@
         <v>72</v>
       </c>
       <c r="B97" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="C97" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="26" t="s">
+      <c r="D97" s="27" t="s">
         <v>221</v>
-      </c>
-      <c r="D97" s="27" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4258,13 +4258,13 @@
         <v>48</v>
       </c>
       <c r="B98" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="C98" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="C98" s="26" t="s">
+      <c r="D98" s="27" t="s">
         <v>218</v>
-      </c>
-      <c r="D98" s="27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4272,7 +4272,7 @@
     </row>
     <row r="100" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="5"/>
@@ -4282,13 +4282,13 @@
         <v>1</v>
       </c>
       <c r="B101" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C101" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="C101" s="32" t="s">
+      <c r="D101" s="33" t="s">
         <v>225</v>
-      </c>
-      <c r="D101" s="33" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,13 +4296,13 @@
         <v>22</v>
       </c>
       <c r="B102" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="C102" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="C102" s="32" t="s">
+      <c r="D102" s="33" t="s">
         <v>228</v>
-      </c>
-      <c r="D102" s="33" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4310,13 +4310,13 @@
         <v>5</v>
       </c>
       <c r="B103" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C103" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="D103" s="33" t="s">
         <v>231</v>
-      </c>
-      <c r="D103" s="33" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4324,13 +4324,13 @@
         <v>8</v>
       </c>
       <c r="B104" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C104" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="C104" s="32" t="s">
+      <c r="D104" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="D104" s="33" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4338,13 +4338,13 @@
         <v>11</v>
       </c>
       <c r="B105" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="C105" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C105" s="32" t="s">
+      <c r="D105" s="33" t="s">
         <v>237</v>
-      </c>
-      <c r="D105" s="33" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4352,13 +4352,13 @@
         <v>14</v>
       </c>
       <c r="B106" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C106" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="D106" s="33" t="s">
         <v>240</v>
-      </c>
-      <c r="D106" s="33" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4366,13 +4366,13 @@
         <v>72</v>
       </c>
       <c r="B107" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C107" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="D107" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="D107" s="33" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4380,13 +4380,13 @@
         <v>48</v>
       </c>
       <c r="B108" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C108" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="C108" s="32" t="s">
+      <c r="D108" s="33" t="s">
         <v>243</v>
-      </c>
-      <c r="D108" s="33" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4396,7 +4396,7 @@
     </row>
     <row r="110" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -4407,13 +4407,13 @@
         <v>1</v>
       </c>
       <c r="B111" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="C111" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="C111" s="39" t="s">
+      <c r="D111" s="40" t="s">
         <v>247</v>
-      </c>
-      <c r="D111" s="40" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4421,13 +4421,13 @@
         <v>22</v>
       </c>
       <c r="B112" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="C112" s="39" t="s">
         <v>249</v>
       </c>
-      <c r="C112" s="39" t="s">
+      <c r="D112" s="40" t="s">
         <v>250</v>
-      </c>
-      <c r="D112" s="40" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4435,13 +4435,13 @@
         <v>5</v>
       </c>
       <c r="B113" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="C113" s="39" t="s">
         <v>252</v>
       </c>
-      <c r="C113" s="39" t="s">
+      <c r="D113" s="40" t="s">
         <v>253</v>
-      </c>
-      <c r="D113" s="40" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4449,27 +4449,27 @@
         <v>8</v>
       </c>
       <c r="B114" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="C114" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="C114" s="39" t="s">
+      <c r="D114" s="40" t="s">
         <v>256</v>
-      </c>
-      <c r="D114" s="40" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="B115" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="B115" s="39" t="s">
+      <c r="C115" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="C115" s="39" t="s">
+      <c r="D115" s="40" t="s">
         <v>260</v>
-      </c>
-      <c r="D115" s="40" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4477,18 +4477,18 @@
         <v>14</v>
       </c>
       <c r="B116" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="C116" s="39" t="s">
         <v>262</v>
       </c>
-      <c r="C116" s="39" t="s">
+      <c r="D116" s="40" t="s">
         <v>263</v>
-      </c>
-      <c r="D116" s="40" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="5"/>
@@ -4498,13 +4498,13 @@
         <v>1</v>
       </c>
       <c r="B119" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C119" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="C119" s="26" t="s">
+      <c r="D119" s="27" t="s">
         <v>267</v>
-      </c>
-      <c r="D119" s="27" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4512,13 +4512,13 @@
         <v>22</v>
       </c>
       <c r="B120" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="C120" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="C120" s="26" t="s">
+      <c r="D120" s="27" t="s">
         <v>270</v>
-      </c>
-      <c r="D120" s="27" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4526,13 +4526,13 @@
         <v>5</v>
       </c>
       <c r="B121" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="C121" s="26" t="s">
         <v>272</v>
       </c>
-      <c r="C121" s="26" t="s">
+      <c r="D121" s="27" t="s">
         <v>273</v>
-      </c>
-      <c r="D121" s="27" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4540,13 +4540,13 @@
         <v>8</v>
       </c>
       <c r="B122" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="C122" s="26" t="s">
         <v>275</v>
       </c>
-      <c r="C122" s="26" t="s">
+      <c r="D122" s="27" t="s">
         <v>276</v>
-      </c>
-      <c r="D122" s="27" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4554,13 +4554,13 @@
         <v>11</v>
       </c>
       <c r="B123" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C123" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="C123" s="26" t="s">
+      <c r="D123" s="27" t="s">
         <v>279</v>
-      </c>
-      <c r="D123" s="27" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4568,13 +4568,13 @@
         <v>14</v>
       </c>
       <c r="B124" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="C124" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="C124" s="26" t="s">
+      <c r="D124" s="41" t="s">
         <v>282</v>
-      </c>
-      <c r="D124" s="41" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4582,13 +4582,13 @@
         <v>72</v>
       </c>
       <c r="B125" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C125" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="C125" s="26" t="s">
+      <c r="D125" s="27" t="s">
         <v>285</v>
-      </c>
-      <c r="D125" s="27" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4596,13 +4596,13 @@
         <v>48</v>
       </c>
       <c r="B126" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="C126" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="C126" s="26" t="s">
+      <c r="D126" s="27" t="s">
         <v>288</v>
-      </c>
-      <c r="D126" s="27" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4610,7 +4610,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D128" s="6"/>
     </row>
@@ -4619,13 +4619,13 @@
         <v>1</v>
       </c>
       <c r="B129" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C129" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="C129" s="26" t="s">
+      <c r="D129" s="26" t="s">
         <v>292</v>
-      </c>
-      <c r="D129" s="26" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4633,13 +4633,13 @@
         <v>22</v>
       </c>
       <c r="B130" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="C130" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="C130" s="26" t="s">
+      <c r="D130" s="26" t="s">
         <v>295</v>
-      </c>
-      <c r="D130" s="26" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -4647,7 +4647,7 @@
         <v>5</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C131" s="26"/>
       <c r="D131" s="27"/>
@@ -4657,13 +4657,13 @@
         <v>8</v>
       </c>
       <c r="B132" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="C132" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="C132" s="26" t="s">
+      <c r="D132" s="26" t="s">
         <v>299</v>
-      </c>
-      <c r="D132" s="26" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,13 +4671,13 @@
         <v>11</v>
       </c>
       <c r="B133" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C133" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="C133" s="26" t="s">
+      <c r="D133" s="26" t="s">
         <v>302</v>
-      </c>
-      <c r="D133" s="26" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
     </row>
     <row r="135" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -4694,28 +4694,28 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>726</v>
+      </c>
+      <c r="C136" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="B136" s="32" t="s">
+      <c r="D136" s="33" t="s">
         <v>727</v>
-      </c>
-      <c r="C136" s="42" t="s">
-        <v>306</v>
-      </c>
-      <c r="D136" s="33" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="26"/>
       <c r="B137" s="32" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C137" s="43">
         <v>0</v>
       </c>
       <c r="D137" s="33" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4723,10 +4723,10 @@
         <v>8</v>
       </c>
       <c r="B138" s="44" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C138" s="63" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D138" s="53">
         <v>0</v>
@@ -4735,7 +4735,7 @@
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="50"/>
       <c r="B139" s="51" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C139" s="52"/>
       <c r="D139" s="54"/>
@@ -4743,7 +4743,7 @@
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="45"/>
       <c r="B140" s="46" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C140" s="47"/>
       <c r="D140" s="48"/>
@@ -4753,11 +4753,11 @@
         <v>8</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C141" s="39"/>
       <c r="D141" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4765,11 +4765,11 @@
         <v>11</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C142" s="39"/>
       <c r="D142" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4777,11 +4777,11 @@
         <v>14</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C143" s="39"/>
       <c r="D143" s="33" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4789,45 +4789,45 @@
         <v>15</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C144" s="26"/>
       <c r="D144" s="33" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="26" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B145" s="32"/>
       <c r="C145" s="26"/>
       <c r="D145" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C146" s="26"/>
       <c r="D146" s="33" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C147" s="26"/>
       <c r="D147" s="33" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,7 +4836,7 @@
     </row>
     <row r="149" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D149" s="7"/>
     </row>
@@ -4845,13 +4845,13 @@
         <v>1</v>
       </c>
       <c r="B150" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="C150" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="C150" s="26" t="s">
+      <c r="D150" s="27" t="s">
         <v>313</v>
-      </c>
-      <c r="D150" s="27" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -4860,7 +4860,7 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="5"/>
@@ -4870,13 +4870,13 @@
         <v>1</v>
       </c>
       <c r="B153" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="C153" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="C153" s="32" t="s">
+      <c r="D153" s="33" t="s">
         <v>316</v>
-      </c>
-      <c r="D153" s="33" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4884,13 +4884,13 @@
         <v>22</v>
       </c>
       <c r="B154" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="C154" s="39" t="s">
         <v>318</v>
       </c>
-      <c r="C154" s="39" t="s">
+      <c r="D154" s="40" t="s">
         <v>319</v>
-      </c>
-      <c r="D154" s="40" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4898,13 +4898,13 @@
         <v>5</v>
       </c>
       <c r="B155" s="39" t="s">
+        <v>320</v>
+      </c>
+      <c r="C155" s="39" t="s">
         <v>321</v>
       </c>
-      <c r="C155" s="39" t="s">
+      <c r="D155" s="40" t="s">
         <v>322</v>
-      </c>
-      <c r="D155" s="40" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4912,13 +4912,13 @@
         <v>8</v>
       </c>
       <c r="B156" s="39" t="s">
+        <v>323</v>
+      </c>
+      <c r="C156" s="39" t="s">
         <v>324</v>
       </c>
-      <c r="C156" s="39" t="s">
+      <c r="D156" s="40" t="s">
         <v>325</v>
-      </c>
-      <c r="D156" s="40" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,13 +4926,13 @@
         <v>11</v>
       </c>
       <c r="B157" s="39" t="s">
+        <v>326</v>
+      </c>
+      <c r="C157" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="C157" s="39" t="s">
+      <c r="D157" s="40" t="s">
         <v>328</v>
-      </c>
-      <c r="D157" s="40" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4940,13 +4940,13 @@
         <v>14</v>
       </c>
       <c r="B158" s="39" t="s">
+        <v>329</v>
+      </c>
+      <c r="C158" s="39" t="s">
         <v>330</v>
       </c>
-      <c r="C158" s="39" t="s">
+      <c r="D158" s="40" t="s">
         <v>331</v>
-      </c>
-      <c r="D158" s="40" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4954,25 +4954,25 @@
         <v>72</v>
       </c>
       <c r="B159" s="39" t="s">
+        <v>332</v>
+      </c>
+      <c r="C159" s="39" t="s">
         <v>333</v>
       </c>
-      <c r="C159" s="39" t="s">
+      <c r="D159" s="40" t="s">
         <v>334</v>
-      </c>
-      <c r="D159" s="40" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="26"/>
       <c r="B160" s="39" t="s">
+        <v>335</v>
+      </c>
+      <c r="C160" s="39" t="s">
         <v>336</v>
       </c>
-      <c r="C160" s="39" t="s">
+      <c r="D160" s="40" t="s">
         <v>337</v>
-      </c>
-      <c r="D160" s="40" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4980,13 +4980,13 @@
         <v>48</v>
       </c>
       <c r="B161" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="C161" s="39" t="s">
         <v>339</v>
       </c>
-      <c r="C161" s="39" t="s">
+      <c r="D161" s="40" t="s">
         <v>340</v>
-      </c>
-      <c r="D161" s="40" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,7 +4996,7 @@
     </row>
     <row r="163" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B163" s="14"/>
       <c r="C163" s="14"/>
@@ -5007,27 +5007,27 @@
         <v>1</v>
       </c>
       <c r="B164" s="39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C164" s="39" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D164" s="40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B165" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="C165" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="C165" s="39" t="s">
+      <c r="D165" s="40" t="s">
         <v>345</v>
-      </c>
-      <c r="D165" s="40" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5035,13 +5035,13 @@
         <v>5</v>
       </c>
       <c r="B166" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="C166" s="39" t="s">
         <v>347</v>
       </c>
-      <c r="C166" s="39" t="s">
+      <c r="D166" s="40" t="s">
         <v>348</v>
-      </c>
-      <c r="D166" s="40" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -5051,7 +5051,7 @@
     </row>
     <row r="168" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B168" s="14"/>
       <c r="C168" s="5"/>
@@ -5061,13 +5061,13 @@
         <v>1</v>
       </c>
       <c r="B169" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="C169" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="C169" s="32" t="s">
+      <c r="D169" s="55" t="s">
         <v>352</v>
-      </c>
-      <c r="D169" s="55" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -5075,13 +5075,13 @@
         <v>22</v>
       </c>
       <c r="B170" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="C170" s="39" t="s">
         <v>354</v>
       </c>
-      <c r="C170" s="39" t="s">
+      <c r="D170" s="56" t="s">
         <v>355</v>
-      </c>
-      <c r="D170" s="56" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5089,11 +5089,11 @@
         <v>5</v>
       </c>
       <c r="B171" s="39" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C171" s="39"/>
       <c r="D171" s="56" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5101,13 +5101,13 @@
         <v>8</v>
       </c>
       <c r="B172" s="39" t="s">
+        <v>358</v>
+      </c>
+      <c r="C172" s="39" t="s">
         <v>359</v>
       </c>
-      <c r="C172" s="39" t="s">
+      <c r="D172" s="56" t="s">
         <v>360</v>
-      </c>
-      <c r="D172" s="56" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5115,13 +5115,13 @@
         <v>11</v>
       </c>
       <c r="B173" s="39" t="s">
+        <v>361</v>
+      </c>
+      <c r="C173" s="39" t="s">
         <v>362</v>
       </c>
-      <c r="C173" s="39" t="s">
+      <c r="D173" s="56" t="s">
         <v>363</v>
-      </c>
-      <c r="D173" s="56" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5129,13 +5129,13 @@
         <v>14</v>
       </c>
       <c r="B174" s="39" t="s">
+        <v>364</v>
+      </c>
+      <c r="C174" s="39" t="s">
         <v>365</v>
       </c>
-      <c r="C174" s="39" t="s">
+      <c r="D174" s="56" t="s">
         <v>366</v>
-      </c>
-      <c r="D174" s="56" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -5143,13 +5143,13 @@
         <v>48</v>
       </c>
       <c r="B175" s="39" t="s">
+        <v>367</v>
+      </c>
+      <c r="C175" s="39" t="s">
         <v>368</v>
       </c>
-      <c r="C175" s="39" t="s">
+      <c r="D175" s="36" t="s">
         <v>369</v>
-      </c>
-      <c r="D175" s="36" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -5159,7 +5159,7 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B177" s="2"/>
       <c r="D177" s="7"/>
@@ -5169,13 +5169,13 @@
         <v>1</v>
       </c>
       <c r="B178" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="C178" s="26" t="s">
         <v>372</v>
       </c>
-      <c r="C178" s="26" t="s">
+      <c r="D178" s="27" t="s">
         <v>373</v>
-      </c>
-      <c r="D178" s="27" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -5183,13 +5183,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="C179" s="26" t="s">
         <v>375</v>
       </c>
-      <c r="C179" s="26" t="s">
+      <c r="D179" s="27" t="s">
         <v>376</v>
-      </c>
-      <c r="D179" s="27" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -5197,13 +5197,13 @@
         <v>5</v>
       </c>
       <c r="B180" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C180" s="26" t="s">
         <v>378</v>
       </c>
-      <c r="C180" s="26" t="s">
+      <c r="D180" s="27" t="s">
         <v>379</v>
-      </c>
-      <c r="D180" s="27" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,13 +5211,13 @@
         <v>8</v>
       </c>
       <c r="B181" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C181" s="26" t="s">
         <v>381</v>
       </c>
-      <c r="C181" s="26" t="s">
+      <c r="D181" s="27" t="s">
         <v>382</v>
-      </c>
-      <c r="D181" s="27" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,13 +5225,13 @@
         <v>11</v>
       </c>
       <c r="B182" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="C182" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="C182" s="26" t="s">
+      <c r="D182" s="27" t="s">
         <v>385</v>
-      </c>
-      <c r="D182" s="27" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -5239,13 +5239,13 @@
         <v>14</v>
       </c>
       <c r="B183" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="C183" s="26" t="s">
         <v>387</v>
       </c>
-      <c r="C183" s="26" t="s">
+      <c r="D183" s="28" t="s">
         <v>388</v>
-      </c>
-      <c r="D183" s="28" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5255,7 +5255,7 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="5"/>
@@ -5265,27 +5265,27 @@
         <v>1</v>
       </c>
       <c r="B186" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="C186" s="26" t="s">
         <v>391</v>
       </c>
-      <c r="C186" s="26" t="s">
+      <c r="D186" s="27" t="s">
         <v>392</v>
-      </c>
-      <c r="D186" s="27" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="B187" s="26" t="s">
         <v>394</v>
       </c>
-      <c r="B187" s="26" t="s">
+      <c r="C187" s="26" t="s">
         <v>395</v>
       </c>
-      <c r="C187" s="26" t="s">
+      <c r="D187" s="27" t="s">
         <v>396</v>
-      </c>
-      <c r="D187" s="27" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,13 +5293,13 @@
         <v>5</v>
       </c>
       <c r="B188" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="C188" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="C188" s="26" t="s">
+      <c r="D188" s="27" t="s">
         <v>399</v>
-      </c>
-      <c r="D188" s="27" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5307,13 +5307,13 @@
         <v>8</v>
       </c>
       <c r="B189" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="C189" s="26" t="s">
         <v>401</v>
       </c>
-      <c r="C189" s="26" t="s">
+      <c r="D189" s="27" t="s">
         <v>402</v>
-      </c>
-      <c r="D189" s="27" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5321,13 +5321,13 @@
         <v>11</v>
       </c>
       <c r="B190" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="C190" s="26" t="s">
         <v>404</v>
       </c>
-      <c r="C190" s="26" t="s">
+      <c r="D190" s="27" t="s">
         <v>405</v>
-      </c>
-      <c r="D190" s="27" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5335,13 +5335,13 @@
         <v>14</v>
       </c>
       <c r="B191" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="C191" s="26" t="s">
         <v>407</v>
       </c>
-      <c r="C191" s="26" t="s">
+      <c r="D191" s="27" t="s">
         <v>408</v>
-      </c>
-      <c r="D191" s="27" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5349,18 +5349,18 @@
         <v>48</v>
       </c>
       <c r="B192" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="C192" s="26" t="s">
         <v>410</v>
       </c>
-      <c r="C192" s="26" t="s">
+      <c r="D192" s="27" t="s">
         <v>411</v>
-      </c>
-      <c r="D192" s="27" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="5"/>
@@ -5370,13 +5370,13 @@
         <v>1</v>
       </c>
       <c r="B195" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="C195" s="26" t="s">
         <v>414</v>
       </c>
-      <c r="C195" s="26" t="s">
+      <c r="D195" s="27" t="s">
         <v>415</v>
-      </c>
-      <c r="D195" s="27" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5384,13 +5384,13 @@
         <v>22</v>
       </c>
       <c r="B196" s="26" t="s">
+        <v>416</v>
+      </c>
+      <c r="C196" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C196" s="26" t="s">
+      <c r="D196" s="27" t="s">
         <v>418</v>
-      </c>
-      <c r="D196" s="27" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5398,13 +5398,13 @@
         <v>5</v>
       </c>
       <c r="B197" s="26" t="s">
+        <v>419</v>
+      </c>
+      <c r="C197" s="26" t="s">
         <v>420</v>
       </c>
-      <c r="C197" s="26" t="s">
+      <c r="D197" s="27" t="s">
         <v>421</v>
-      </c>
-      <c r="D197" s="27" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5412,13 +5412,13 @@
         <v>8</v>
       </c>
       <c r="B198" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="C198" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="C198" s="26" t="s">
+      <c r="D198" s="27" t="s">
         <v>424</v>
-      </c>
-      <c r="D198" s="27" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5426,18 +5426,18 @@
         <v>14</v>
       </c>
       <c r="B199" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="C199" s="26" t="s">
         <v>426</v>
       </c>
-      <c r="C199" s="26" t="s">
+      <c r="D199" s="27" t="s">
         <v>427</v>
-      </c>
-      <c r="D199" s="27" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
@@ -5447,13 +5447,13 @@
         <v>1</v>
       </c>
       <c r="B202" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="C202" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="C202" s="26" t="s">
+      <c r="D202" s="27" t="s">
         <v>431</v>
-      </c>
-      <c r="D202" s="27" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5461,13 +5461,13 @@
         <v>22</v>
       </c>
       <c r="B203" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="C203" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="C203" s="26" t="s">
+      <c r="D203" s="27" t="s">
         <v>434</v>
-      </c>
-      <c r="D203" s="27" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5475,13 +5475,13 @@
         <v>5</v>
       </c>
       <c r="B204" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="C204" s="26" t="s">
         <v>436</v>
       </c>
-      <c r="C204" s="26" t="s">
+      <c r="D204" s="27" t="s">
         <v>437</v>
-      </c>
-      <c r="D204" s="27" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5489,13 +5489,13 @@
         <v>8</v>
       </c>
       <c r="B205" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="C205" s="26" t="s">
         <v>439</v>
       </c>
-      <c r="C205" s="26" t="s">
+      <c r="D205" s="27" t="s">
         <v>440</v>
-      </c>
-      <c r="D205" s="27" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5503,13 +5503,13 @@
         <v>11</v>
       </c>
       <c r="B206" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="C206" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="C206" s="26" t="s">
+      <c r="D206" s="27" t="s">
         <v>443</v>
-      </c>
-      <c r="D206" s="27" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5517,13 +5517,13 @@
         <v>14</v>
       </c>
       <c r="B207" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="C207" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="C207" s="26" t="s">
+      <c r="D207" s="27" t="s">
         <v>443</v>
-      </c>
-      <c r="D207" s="27" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5531,7 +5531,7 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D209" s="7"/>
     </row>
@@ -5540,13 +5540,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="C210" s="26" t="s">
         <v>446</v>
       </c>
-      <c r="C210" s="26" t="s">
+      <c r="D210" s="27" t="s">
         <v>447</v>
-      </c>
-      <c r="D210" s="27" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5554,13 +5554,13 @@
         <v>22</v>
       </c>
       <c r="B211" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="C211" s="26" t="s">
         <v>449</v>
       </c>
-      <c r="C211" s="26" t="s">
+      <c r="D211" s="27" t="s">
         <v>450</v>
-      </c>
-      <c r="D211" s="27" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5568,11 +5568,11 @@
         <v>5</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C212" s="26"/>
       <c r="D212" s="27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5588,11 +5588,11 @@
         <v>14</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C214" s="26"/>
       <c r="D214" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5600,11 +5600,11 @@
         <v>15</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C215" s="26"/>
       <c r="D215" s="27" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5612,13 +5612,13 @@
         <v>68</v>
       </c>
       <c r="B216" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="C216" s="26" t="s">
         <v>458</v>
       </c>
-      <c r="C216" s="26" t="s">
+      <c r="D216" s="27" t="s">
         <v>459</v>
-      </c>
-      <c r="D216" s="27" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5626,13 +5626,13 @@
         <v>72</v>
       </c>
       <c r="B217" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="C217" s="26" t="s">
         <v>461</v>
       </c>
-      <c r="C217" s="26" t="s">
+      <c r="D217" s="27" t="s">
         <v>462</v>
-      </c>
-      <c r="D217" s="27" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5640,13 +5640,13 @@
         <v>48</v>
       </c>
       <c r="B218" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="C218" s="26" t="s">
         <v>464</v>
       </c>
-      <c r="C218" s="26" t="s">
+      <c r="D218" s="27" t="s">
         <v>465</v>
-      </c>
-      <c r="D218" s="27" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5655,7 +5655,7 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D220" s="7"/>
     </row>
@@ -5664,13 +5664,13 @@
         <v>1</v>
       </c>
       <c r="B221" s="26" t="s">
+        <v>467</v>
+      </c>
+      <c r="C221" s="26" t="s">
         <v>468</v>
       </c>
-      <c r="C221" s="26" t="s">
+      <c r="D221" s="27" t="s">
         <v>469</v>
-      </c>
-      <c r="D221" s="27" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5678,13 +5678,13 @@
         <v>22</v>
       </c>
       <c r="B222" s="26" t="s">
+        <v>470</v>
+      </c>
+      <c r="C222" s="26" t="s">
         <v>471</v>
       </c>
-      <c r="C222" s="26" t="s">
+      <c r="D222" s="27" t="s">
         <v>472</v>
-      </c>
-      <c r="D222" s="27" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5692,13 +5692,13 @@
         <v>5</v>
       </c>
       <c r="B223" s="26" t="s">
+        <v>473</v>
+      </c>
+      <c r="C223" s="26" t="s">
         <v>474</v>
       </c>
-      <c r="C223" s="26" t="s">
+      <c r="D223" s="27" t="s">
         <v>475</v>
-      </c>
-      <c r="D223" s="27" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5706,13 +5706,13 @@
         <v>8</v>
       </c>
       <c r="B224" s="26" t="s">
+        <v>473</v>
+      </c>
+      <c r="C224" s="26" t="s">
         <v>474</v>
       </c>
-      <c r="C224" s="26" t="s">
+      <c r="D224" s="27" t="s">
         <v>475</v>
-      </c>
-      <c r="D224" s="27" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5720,13 +5720,13 @@
         <v>11</v>
       </c>
       <c r="B225" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="C225" s="26" t="s">
         <v>477</v>
       </c>
-      <c r="C225" s="26" t="s">
+      <c r="D225" s="27" t="s">
         <v>478</v>
-      </c>
-      <c r="D225" s="27" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5734,13 +5734,13 @@
         <v>14</v>
       </c>
       <c r="B226" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="C226" s="26" t="s">
         <v>477</v>
       </c>
-      <c r="C226" s="26" t="s">
+      <c r="D226" s="27" t="s">
         <v>478</v>
-      </c>
-      <c r="D226" s="27" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5748,13 +5748,13 @@
         <v>68</v>
       </c>
       <c r="B227" s="26" t="s">
+        <v>479</v>
+      </c>
+      <c r="C227" s="26" t="s">
         <v>480</v>
       </c>
-      <c r="C227" s="26" t="s">
+      <c r="D227" s="27" t="s">
         <v>481</v>
-      </c>
-      <c r="D227" s="27" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5775,16 +5775,16 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B230" s="26" t="s">
+        <v>470</v>
+      </c>
+      <c r="C230" s="26" t="s">
         <v>471</v>
       </c>
-      <c r="C230" s="26" t="s">
+      <c r="D230" s="57" t="s">
         <v>472</v>
-      </c>
-      <c r="D230" s="57" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5792,7 +5792,7 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B232" s="4"/>
       <c r="C232" s="5"/>
@@ -5802,13 +5802,13 @@
         <v>1</v>
       </c>
       <c r="B233" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="C233" s="26" t="s">
         <v>484</v>
       </c>
-      <c r="C233" s="26" t="s">
+      <c r="D233" s="27" t="s">
         <v>485</v>
-      </c>
-      <c r="D233" s="27" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5816,13 +5816,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="26" t="s">
+        <v>486</v>
+      </c>
+      <c r="C234" s="26" t="s">
         <v>487</v>
       </c>
-      <c r="C234" s="26" t="s">
+      <c r="D234" s="27" t="s">
         <v>488</v>
-      </c>
-      <c r="D234" s="27" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5830,13 +5830,13 @@
         <v>5</v>
       </c>
       <c r="B235" s="26" t="s">
+        <v>489</v>
+      </c>
+      <c r="C235" s="26" t="s">
         <v>490</v>
       </c>
-      <c r="C235" s="26" t="s">
+      <c r="D235" s="27" t="s">
         <v>491</v>
-      </c>
-      <c r="D235" s="27" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5844,11 +5844,11 @@
         <v>8</v>
       </c>
       <c r="B236" s="26" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C236" s="26"/>
       <c r="D236" s="27" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5864,11 +5864,11 @@
         <v>14</v>
       </c>
       <c r="B238" s="26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C238" s="26"/>
       <c r="D238" s="27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -5876,11 +5876,11 @@
         <v>15</v>
       </c>
       <c r="B239" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C239" s="26"/>
       <c r="D239" s="27" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -5888,13 +5888,13 @@
         <v>68</v>
       </c>
       <c r="B240" s="26" t="s">
+        <v>498</v>
+      </c>
+      <c r="C240" s="26" t="s">
         <v>499</v>
       </c>
-      <c r="C240" s="26" t="s">
+      <c r="D240" s="27" t="s">
         <v>500</v>
-      </c>
-      <c r="D240" s="27" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5902,13 +5902,13 @@
         <v>72</v>
       </c>
       <c r="B241" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="C241" s="26" t="s">
         <v>484</v>
       </c>
-      <c r="C241" s="26" t="s">
+      <c r="D241" s="27" t="s">
         <v>485</v>
-      </c>
-      <c r="D241" s="27" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5916,16 +5916,16 @@
         <v>48</v>
       </c>
       <c r="B242" s="26" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C242" s="26"/>
       <c r="D242" s="27" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="5"/>
@@ -5935,13 +5935,13 @@
         <v>1</v>
       </c>
       <c r="B245" s="58" t="s">
+        <v>504</v>
+      </c>
+      <c r="C245" s="58" t="s">
         <v>505</v>
       </c>
-      <c r="C245" s="58" t="s">
+      <c r="D245" s="59" t="s">
         <v>506</v>
-      </c>
-      <c r="D245" s="59" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -5949,13 +5949,13 @@
         <v>22</v>
       </c>
       <c r="B246" s="26" t="s">
+        <v>507</v>
+      </c>
+      <c r="C246" s="26" t="s">
         <v>508</v>
       </c>
-      <c r="C246" s="26" t="s">
+      <c r="D246" s="27" t="s">
         <v>509</v>
-      </c>
-      <c r="D246" s="27" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -5963,13 +5963,13 @@
         <v>5</v>
       </c>
       <c r="B247" s="26" t="s">
+        <v>510</v>
+      </c>
+      <c r="C247" s="26" t="s">
         <v>511</v>
       </c>
-      <c r="C247" s="26" t="s">
+      <c r="D247" s="28" t="s">
         <v>512</v>
-      </c>
-      <c r="D247" s="28" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5977,13 +5977,13 @@
         <v>8</v>
       </c>
       <c r="B248" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="C248" s="26" t="s">
         <v>514</v>
       </c>
-      <c r="C248" s="26" t="s">
+      <c r="D248" s="28" t="s">
         <v>515</v>
-      </c>
-      <c r="D248" s="28" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -5991,13 +5991,13 @@
         <v>11</v>
       </c>
       <c r="B249" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="C249" s="26" t="s">
         <v>517</v>
       </c>
-      <c r="C249" s="26" t="s">
+      <c r="D249" s="28" t="s">
         <v>518</v>
-      </c>
-      <c r="D249" s="28" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -6005,13 +6005,13 @@
         <v>14</v>
       </c>
       <c r="B250" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="C250" s="26" t="s">
         <v>517</v>
       </c>
-      <c r="C250" s="26" t="s">
+      <c r="D250" s="28" t="s">
         <v>518</v>
-      </c>
-      <c r="D250" s="28" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -6019,18 +6019,18 @@
         <v>68</v>
       </c>
       <c r="B251" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="C251" s="60" t="s">
         <v>520</v>
       </c>
-      <c r="C251" s="60" t="s">
+      <c r="D251" s="28" t="s">
         <v>521</v>
-      </c>
-      <c r="D251" s="28" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="5"/>
@@ -6040,13 +6040,13 @@
         <v>1</v>
       </c>
       <c r="B254" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="C254" s="26" t="s">
         <v>524</v>
       </c>
-      <c r="C254" s="26" t="s">
+      <c r="D254" s="27" t="s">
         <v>525</v>
-      </c>
-      <c r="D254" s="27" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -6054,13 +6054,13 @@
         <v>22</v>
       </c>
       <c r="B255" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="C255" s="26" t="s">
         <v>527</v>
       </c>
-      <c r="C255" s="26" t="s">
+      <c r="D255" s="27" t="s">
         <v>528</v>
-      </c>
-      <c r="D255" s="27" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -6068,13 +6068,13 @@
         <v>5</v>
       </c>
       <c r="B256" s="26" t="s">
+        <v>529</v>
+      </c>
+      <c r="C256" s="26" t="s">
         <v>530</v>
       </c>
-      <c r="C256" s="26" t="s">
+      <c r="D256" s="27" t="s">
         <v>531</v>
-      </c>
-      <c r="D256" s="27" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -6082,13 +6082,13 @@
         <v>8</v>
       </c>
       <c r="B257" s="26" t="s">
+        <v>532</v>
+      </c>
+      <c r="C257" s="26" t="s">
         <v>533</v>
       </c>
-      <c r="C257" s="26" t="s">
+      <c r="D257" s="27" t="s">
         <v>534</v>
-      </c>
-      <c r="D257" s="27" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -6096,13 +6096,13 @@
         <v>11</v>
       </c>
       <c r="B258" s="26" t="s">
+        <v>535</v>
+      </c>
+      <c r="C258" s="26" t="s">
         <v>536</v>
       </c>
-      <c r="C258" s="26" t="s">
+      <c r="D258" s="27" t="s">
         <v>537</v>
-      </c>
-      <c r="D258" s="27" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,13 +6110,13 @@
         <v>14</v>
       </c>
       <c r="B259" s="26" t="s">
+        <v>538</v>
+      </c>
+      <c r="C259" s="26" t="s">
         <v>539</v>
       </c>
-      <c r="C259" s="26" t="s">
+      <c r="D259" s="27" t="s">
         <v>540</v>
-      </c>
-      <c r="D259" s="27" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -6124,13 +6124,13 @@
         <v>68</v>
       </c>
       <c r="B260" s="26" t="s">
+        <v>541</v>
+      </c>
+      <c r="C260" s="26" t="s">
         <v>542</v>
       </c>
-      <c r="C260" s="26" t="s">
+      <c r="D260" s="27" t="s">
         <v>543</v>
-      </c>
-      <c r="D260" s="27" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -6138,13 +6138,13 @@
         <v>72</v>
       </c>
       <c r="B261" s="26" t="s">
+        <v>544</v>
+      </c>
+      <c r="C261" s="26" t="s">
         <v>545</v>
       </c>
-      <c r="C261" s="26" t="s">
+      <c r="D261" s="27" t="s">
         <v>546</v>
-      </c>
-      <c r="D261" s="27" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -6152,46 +6152,46 @@
         <v>48</v>
       </c>
       <c r="B262" s="26" t="s">
+        <v>547</v>
+      </c>
+      <c r="C262" s="26" t="s">
         <v>548</v>
       </c>
-      <c r="C262" s="26" t="s">
+      <c r="D262" s="27" t="s">
         <v>549</v>
-      </c>
-      <c r="D262" s="27" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B263" s="26" t="s">
+        <v>550</v>
+      </c>
+      <c r="C263" s="26" t="s">
         <v>551</v>
       </c>
-      <c r="C263" s="26" t="s">
+      <c r="D263" s="27" t="s">
         <v>552</v>
-      </c>
-      <c r="D263" s="27" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="26" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B264" s="26" t="s">
+        <v>550</v>
+      </c>
+      <c r="C264" s="26" t="s">
         <v>551</v>
       </c>
-      <c r="C264" s="26" t="s">
+      <c r="D264" s="27" t="s">
         <v>552</v>
-      </c>
-      <c r="D264" s="27" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="5"/>
@@ -6201,13 +6201,13 @@
         <v>1</v>
       </c>
       <c r="B267" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="C267" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="C267" s="26" t="s">
+      <c r="D267" s="27" t="s">
         <v>557</v>
-      </c>
-      <c r="D267" s="27" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,13 +6215,13 @@
         <v>22</v>
       </c>
       <c r="B268" s="26" t="s">
+        <v>558</v>
+      </c>
+      <c r="C268" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="C268" s="26" t="s">
+      <c r="D268" s="27" t="s">
         <v>560</v>
-      </c>
-      <c r="D268" s="27" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -6229,13 +6229,13 @@
         <v>5</v>
       </c>
       <c r="B269" s="26" t="s">
+        <v>558</v>
+      </c>
+      <c r="C269" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="C269" s="26" t="s">
+      <c r="D269" s="27" t="s">
         <v>560</v>
-      </c>
-      <c r="D269" s="27" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -6243,13 +6243,13 @@
         <v>8</v>
       </c>
       <c r="B270" s="26" t="s">
+        <v>561</v>
+      </c>
+      <c r="C270" s="26" t="s">
         <v>562</v>
       </c>
-      <c r="C270" s="26" t="s">
+      <c r="D270" s="27" t="s">
         <v>563</v>
-      </c>
-      <c r="D270" s="27" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6257,13 +6257,13 @@
         <v>11</v>
       </c>
       <c r="B271" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="C271" s="26" t="s">
         <v>565</v>
       </c>
-      <c r="C271" s="26" t="s">
+      <c r="D271" s="27" t="s">
         <v>566</v>
-      </c>
-      <c r="D271" s="27" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -6271,13 +6271,13 @@
         <v>14</v>
       </c>
       <c r="B272" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="C272" s="26" t="s">
         <v>565</v>
       </c>
-      <c r="C272" s="26" t="s">
+      <c r="D272" s="27" t="s">
         <v>566</v>
-      </c>
-      <c r="D272" s="27" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -6285,13 +6285,13 @@
         <v>15</v>
       </c>
       <c r="B273" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="C273" s="26" t="s">
         <v>565</v>
       </c>
-      <c r="C273" s="26" t="s">
+      <c r="D273" s="27" t="s">
         <v>566</v>
-      </c>
-      <c r="D273" s="27" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6299,13 +6299,13 @@
         <v>72</v>
       </c>
       <c r="B274" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="C274" s="26" t="s">
         <v>568</v>
       </c>
-      <c r="C274" s="26" t="s">
+      <c r="D274" s="27" t="s">
         <v>569</v>
-      </c>
-      <c r="D274" s="27" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -6313,18 +6313,18 @@
         <v>48</v>
       </c>
       <c r="B275" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="C275" s="26" t="s">
         <v>568</v>
       </c>
-      <c r="C275" s="26" t="s">
+      <c r="D275" s="27" t="s">
         <v>569</v>
-      </c>
-      <c r="D275" s="27" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A277" s="13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="5"/>
@@ -6334,13 +6334,13 @@
         <v>1</v>
       </c>
       <c r="B278" s="26" t="s">
+        <v>571</v>
+      </c>
+      <c r="C278" s="26" t="s">
         <v>572</v>
       </c>
-      <c r="C278" s="26" t="s">
+      <c r="D278" s="61" t="s">
         <v>573</v>
-      </c>
-      <c r="D278" s="61" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -6348,13 +6348,13 @@
         <v>22</v>
       </c>
       <c r="B279" s="26" t="s">
+        <v>574</v>
+      </c>
+      <c r="C279" s="26" t="s">
         <v>575</v>
       </c>
-      <c r="C279" s="26" t="s">
+      <c r="D279" s="61" t="s">
         <v>576</v>
-      </c>
-      <c r="D279" s="61" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -6362,13 +6362,13 @@
         <v>5</v>
       </c>
       <c r="B280" s="26" t="s">
+        <v>577</v>
+      </c>
+      <c r="C280" s="26" t="s">
         <v>578</v>
       </c>
-      <c r="C280" s="26" t="s">
+      <c r="D280" s="28" t="s">
         <v>579</v>
-      </c>
-      <c r="D280" s="28" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -6376,13 +6376,13 @@
         <v>8</v>
       </c>
       <c r="B281" s="26" t="s">
+        <v>580</v>
+      </c>
+      <c r="C281" s="26" t="s">
         <v>581</v>
       </c>
-      <c r="C281" s="26" t="s">
+      <c r="D281" s="61" t="s">
         <v>582</v>
-      </c>
-      <c r="D281" s="61" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -6390,13 +6390,13 @@
         <v>11</v>
       </c>
       <c r="B282" s="26" t="s">
+        <v>583</v>
+      </c>
+      <c r="C282" s="26" t="s">
         <v>584</v>
       </c>
-      <c r="C282" s="26" t="s">
+      <c r="D282" s="28" t="s">
         <v>585</v>
-      </c>
-      <c r="D282" s="28" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -6404,13 +6404,13 @@
         <v>14</v>
       </c>
       <c r="B283" s="26" t="s">
+        <v>586</v>
+      </c>
+      <c r="C283" s="26" t="s">
         <v>587</v>
       </c>
-      <c r="C283" s="26" t="s">
+      <c r="D283" s="28" t="s">
         <v>588</v>
-      </c>
-      <c r="D283" s="28" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -6426,18 +6426,18 @@
         <v>48</v>
       </c>
       <c r="B285" s="26" t="s">
+        <v>589</v>
+      </c>
+      <c r="C285" s="26" t="s">
         <v>590</v>
       </c>
-      <c r="C285" s="26" t="s">
+      <c r="D285" s="61" t="s">
         <v>591</v>
-      </c>
-      <c r="D285" s="61" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -6447,13 +6447,13 @@
         <v>1</v>
       </c>
       <c r="B288" s="26" t="s">
+        <v>593</v>
+      </c>
+      <c r="C288" s="26" t="s">
         <v>594</v>
       </c>
-      <c r="C288" s="26" t="s">
+      <c r="D288" s="27" t="s">
         <v>595</v>
-      </c>
-      <c r="D288" s="27" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6461,13 +6461,13 @@
         <v>22</v>
       </c>
       <c r="B289" s="26" t="s">
+        <v>596</v>
+      </c>
+      <c r="C289" s="26" t="s">
         <v>597</v>
       </c>
-      <c r="C289" s="26" t="s">
+      <c r="D289" s="27" t="s">
         <v>598</v>
-      </c>
-      <c r="D289" s="27" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6475,13 +6475,13 @@
         <v>5</v>
       </c>
       <c r="B290" s="26" t="s">
+        <v>599</v>
+      </c>
+      <c r="C290" s="26" t="s">
         <v>600</v>
       </c>
-      <c r="C290" s="26" t="s">
+      <c r="D290" s="27" t="s">
         <v>601</v>
-      </c>
-      <c r="D290" s="27" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -6489,13 +6489,13 @@
         <v>8</v>
       </c>
       <c r="B291" s="26" t="s">
+        <v>602</v>
+      </c>
+      <c r="C291" s="26" t="s">
         <v>603</v>
       </c>
-      <c r="C291" s="26" t="s">
+      <c r="D291" s="27" t="s">
         <v>604</v>
-      </c>
-      <c r="D291" s="27" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -6503,13 +6503,13 @@
         <v>11</v>
       </c>
       <c r="B292" s="26" t="s">
+        <v>605</v>
+      </c>
+      <c r="C292" s="26" t="s">
         <v>606</v>
       </c>
-      <c r="C292" s="26" t="s">
+      <c r="D292" s="27" t="s">
         <v>607</v>
-      </c>
-      <c r="D292" s="27" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -6517,27 +6517,27 @@
         <v>14</v>
       </c>
       <c r="B293" s="26" t="s">
+        <v>608</v>
+      </c>
+      <c r="C293" s="26" t="s">
         <v>609</v>
       </c>
-      <c r="C293" s="26" t="s">
+      <c r="D293" s="27" t="s">
         <v>610</v>
-      </c>
-      <c r="D293" s="27" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="26" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B294" s="26" t="s">
+        <v>611</v>
+      </c>
+      <c r="C294" s="26" t="s">
         <v>612</v>
       </c>
-      <c r="C294" s="26" t="s">
+      <c r="D294" s="27" t="s">
         <v>613</v>
-      </c>
-      <c r="D294" s="27" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -6545,7 +6545,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="22" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B296" s="5"/>
       <c r="D296" s="7"/>
@@ -6555,13 +6555,13 @@
         <v>1</v>
       </c>
       <c r="B297" s="26" t="s">
+        <v>615</v>
+      </c>
+      <c r="C297" s="26" t="s">
         <v>616</v>
       </c>
-      <c r="C297" s="26" t="s">
+      <c r="D297" s="26" t="s">
         <v>617</v>
-      </c>
-      <c r="D297" s="26" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -6569,13 +6569,13 @@
         <v>22</v>
       </c>
       <c r="B298" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="C298" s="26" t="s">
         <v>619</v>
       </c>
-      <c r="C298" s="26" t="s">
+      <c r="D298" s="26" t="s">
         <v>620</v>
-      </c>
-      <c r="D298" s="26" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -6583,13 +6583,13 @@
         <v>5</v>
       </c>
       <c r="B299" s="26" t="s">
+        <v>621</v>
+      </c>
+      <c r="C299" s="26" t="s">
         <v>622</v>
       </c>
-      <c r="C299" s="26" t="s">
+      <c r="D299" s="26" t="s">
         <v>623</v>
-      </c>
-      <c r="D299" s="26" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -6597,13 +6597,13 @@
         <v>8</v>
       </c>
       <c r="B300" s="26" t="s">
+        <v>624</v>
+      </c>
+      <c r="C300" s="26" t="s">
         <v>625</v>
       </c>
-      <c r="C300" s="26" t="s">
+      <c r="D300" s="26" t="s">
         <v>626</v>
-      </c>
-      <c r="D300" s="26" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -6611,25 +6611,25 @@
         <v>11</v>
       </c>
       <c r="B301" s="26" t="s">
+        <v>627</v>
+      </c>
+      <c r="C301" s="26" t="s">
         <v>628</v>
       </c>
-      <c r="C301" s="26" t="s">
+      <c r="D301" s="26" t="s">
         <v>629</v>
-      </c>
-      <c r="D301" s="26" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="26"/>
       <c r="B302" s="26" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C302" s="26" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D302" s="26" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -6637,7 +6637,7 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A304" s="23" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
@@ -6647,13 +6647,13 @@
         <v>1</v>
       </c>
       <c r="B305" s="26" t="s">
+        <v>632</v>
+      </c>
+      <c r="C305" s="26" t="s">
         <v>633</v>
       </c>
-      <c r="C305" s="26" t="s">
+      <c r="D305" s="27" t="s">
         <v>634</v>
-      </c>
-      <c r="D305" s="27" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -6661,13 +6661,13 @@
         <v>22</v>
       </c>
       <c r="B306" s="26" t="s">
+        <v>635</v>
+      </c>
+      <c r="C306" s="26" t="s">
         <v>636</v>
       </c>
-      <c r="C306" s="26" t="s">
+      <c r="D306" s="27" t="s">
         <v>637</v>
-      </c>
-      <c r="D306" s="27" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -6675,13 +6675,13 @@
         <v>5</v>
       </c>
       <c r="B307" s="26" t="s">
+        <v>638</v>
+      </c>
+      <c r="C307" s="26" t="s">
         <v>639</v>
       </c>
-      <c r="C307" s="26" t="s">
+      <c r="D307" s="27" t="s">
         <v>640</v>
-      </c>
-      <c r="D307" s="27" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -6689,13 +6689,13 @@
         <v>8</v>
       </c>
       <c r="B308" s="26" t="s">
+        <v>641</v>
+      </c>
+      <c r="C308" s="26" t="s">
         <v>642</v>
       </c>
-      <c r="C308" s="26" t="s">
+      <c r="D308" s="27" t="s">
         <v>643</v>
-      </c>
-      <c r="D308" s="27" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -6703,13 +6703,13 @@
         <v>11</v>
       </c>
       <c r="B309" s="26" t="s">
+        <v>644</v>
+      </c>
+      <c r="C309" s="26" t="s">
         <v>645</v>
       </c>
-      <c r="C309" s="26" t="s">
+      <c r="D309" s="27" t="s">
         <v>646</v>
-      </c>
-      <c r="D309" s="27" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -6717,13 +6717,13 @@
         <v>14</v>
       </c>
       <c r="B310" s="26" t="s">
+        <v>647</v>
+      </c>
+      <c r="C310" s="26" t="s">
         <v>648</v>
       </c>
-      <c r="C310" s="26" t="s">
+      <c r="D310" s="27" t="s">
         <v>649</v>
-      </c>
-      <c r="D310" s="27" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -6731,13 +6731,13 @@
         <v>68</v>
       </c>
       <c r="B311" s="26" t="s">
+        <v>650</v>
+      </c>
+      <c r="C311" s="26" t="s">
         <v>651</v>
       </c>
-      <c r="C311" s="26" t="s">
+      <c r="D311" s="27" t="s">
         <v>652</v>
-      </c>
-      <c r="D311" s="27" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -6745,13 +6745,13 @@
         <v>72</v>
       </c>
       <c r="B312" s="26" t="s">
+        <v>653</v>
+      </c>
+      <c r="C312" s="26" t="s">
         <v>654</v>
       </c>
-      <c r="C312" s="26" t="s">
+      <c r="D312" s="27" t="s">
         <v>655</v>
-      </c>
-      <c r="D312" s="27" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -6759,7 +6759,7 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A314" s="8" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D314" s="21"/>
     </row>
@@ -6768,23 +6768,23 @@
         <v>1</v>
       </c>
       <c r="B315" s="26" t="s">
+        <v>657</v>
+      </c>
+      <c r="C315" s="26" t="s">
         <v>658</v>
       </c>
-      <c r="C315" s="26" t="s">
+      <c r="D315" s="27" t="s">
         <v>659</v>
-      </c>
-      <c r="D315" s="27" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="26"/>
       <c r="B316" s="26" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C316" s="26"/>
       <c r="D316" s="27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -6792,13 +6792,13 @@
         <v>22</v>
       </c>
       <c r="B317" s="26" t="s">
+        <v>662</v>
+      </c>
+      <c r="C317" s="26" t="s">
         <v>663</v>
       </c>
-      <c r="C317" s="26" t="s">
+      <c r="D317" s="27" t="s">
         <v>664</v>
-      </c>
-      <c r="D317" s="27" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -6806,13 +6806,13 @@
         <v>5</v>
       </c>
       <c r="B318" s="26" t="s">
+        <v>665</v>
+      </c>
+      <c r="C318" s="26" t="s">
         <v>666</v>
       </c>
-      <c r="C318" s="26" t="s">
+      <c r="D318" s="27" t="s">
         <v>667</v>
-      </c>
-      <c r="D318" s="27" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -6820,13 +6820,13 @@
         <v>8</v>
       </c>
       <c r="B319" s="26" t="s">
+        <v>739</v>
+      </c>
+      <c r="C319" s="26" t="s">
+        <v>666</v>
+      </c>
+      <c r="D319" s="61" t="s">
         <v>740</v>
-      </c>
-      <c r="C319" s="26" t="s">
-        <v>667</v>
-      </c>
-      <c r="D319" s="61" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -6834,13 +6834,13 @@
         <v>11</v>
       </c>
       <c r="B320" s="26" t="s">
+        <v>668</v>
+      </c>
+      <c r="C320" s="26" t="s">
         <v>669</v>
       </c>
-      <c r="C320" s="26" t="s">
+      <c r="D320" s="27" t="s">
         <v>670</v>
-      </c>
-      <c r="D320" s="27" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -6848,18 +6848,18 @@
         <v>14</v>
       </c>
       <c r="B321" s="26" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C321" s="26" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D321" s="27" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A323" s="13" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="5"/>
@@ -6869,13 +6869,13 @@
         <v>1</v>
       </c>
       <c r="B324" s="26" t="s">
+        <v>673</v>
+      </c>
+      <c r="C324" s="26" t="s">
         <v>674</v>
       </c>
-      <c r="C324" s="26" t="s">
+      <c r="D324" s="27" t="s">
         <v>675</v>
-      </c>
-      <c r="D324" s="27" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -6883,13 +6883,13 @@
         <v>5</v>
       </c>
       <c r="B325" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="C325" s="26" t="s">
         <v>677</v>
       </c>
-      <c r="C325" s="26" t="s">
+      <c r="D325" s="27" t="s">
         <v>678</v>
-      </c>
-      <c r="D325" s="27" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -6897,13 +6897,13 @@
         <v>8</v>
       </c>
       <c r="B326" s="26" t="s">
+        <v>679</v>
+      </c>
+      <c r="C326" s="26" t="s">
         <v>680</v>
       </c>
-      <c r="C326" s="26" t="s">
+      <c r="D326" s="27" t="s">
         <v>681</v>
-      </c>
-      <c r="D326" s="27" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -6911,13 +6911,13 @@
         <v>11</v>
       </c>
       <c r="B327" s="26" t="s">
+        <v>682</v>
+      </c>
+      <c r="C327" s="26" t="s">
         <v>683</v>
       </c>
-      <c r="C327" s="26" t="s">
+      <c r="D327" s="27" t="s">
         <v>684</v>
-      </c>
-      <c r="D327" s="27" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6925,13 +6925,13 @@
         <v>14</v>
       </c>
       <c r="B328" s="26" t="s">
+        <v>682</v>
+      </c>
+      <c r="C328" s="26" t="s">
         <v>683</v>
       </c>
-      <c r="C328" s="26" t="s">
+      <c r="D328" s="27" t="s">
         <v>684</v>
-      </c>
-      <c r="D328" s="27" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -6939,13 +6939,13 @@
         <v>68</v>
       </c>
       <c r="B329" s="26" t="s">
+        <v>682</v>
+      </c>
+      <c r="C329" s="26" t="s">
         <v>683</v>
       </c>
-      <c r="C329" s="26" t="s">
+      <c r="D329" s="27" t="s">
         <v>684</v>
-      </c>
-      <c r="D329" s="27" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -6953,18 +6953,18 @@
         <v>72</v>
       </c>
       <c r="B330" s="26" t="s">
+        <v>685</v>
+      </c>
+      <c r="C330" s="26" t="s">
         <v>686</v>
       </c>
-      <c r="C330" s="26" t="s">
+      <c r="D330" s="27" t="s">
         <v>687</v>
-      </c>
-      <c r="D330" s="27" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A332" s="13" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B332" s="24"/>
       <c r="C332" s="25"/>
@@ -6974,13 +6974,13 @@
         <v>1</v>
       </c>
       <c r="B333" s="62" t="s">
+        <v>689</v>
+      </c>
+      <c r="C333" s="62" t="s">
         <v>690</v>
       </c>
-      <c r="C333" s="62" t="s">
+      <c r="D333" s="57" t="s">
         <v>691</v>
-      </c>
-      <c r="D333" s="57" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -6988,13 +6988,13 @@
         <v>22</v>
       </c>
       <c r="B334" s="62" t="s">
+        <v>692</v>
+      </c>
+      <c r="C334" s="62" t="s">
         <v>693</v>
       </c>
-      <c r="C334" s="62" t="s">
+      <c r="D334" s="57" t="s">
         <v>694</v>
-      </c>
-      <c r="D334" s="57" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -7002,13 +7002,13 @@
         <v>5</v>
       </c>
       <c r="B335" s="62" t="s">
+        <v>695</v>
+      </c>
+      <c r="C335" s="62" t="s">
         <v>696</v>
       </c>
-      <c r="C335" s="62" t="s">
+      <c r="D335" s="57" t="s">
         <v>697</v>
-      </c>
-      <c r="D335" s="57" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -7016,13 +7016,13 @@
         <v>8</v>
       </c>
       <c r="B336" s="62" t="s">
+        <v>698</v>
+      </c>
+      <c r="C336" s="62" t="s">
         <v>699</v>
       </c>
-      <c r="C336" s="62" t="s">
+      <c r="D336" s="57" t="s">
         <v>700</v>
-      </c>
-      <c r="D336" s="57" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -7030,13 +7030,13 @@
         <v>11</v>
       </c>
       <c r="B337" s="62" t="s">
+        <v>701</v>
+      </c>
+      <c r="C337" s="62" t="s">
         <v>702</v>
       </c>
-      <c r="C337" s="62" t="s">
+      <c r="D337" s="57" t="s">
         <v>703</v>
-      </c>
-      <c r="D337" s="57" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -7044,13 +7044,13 @@
         <v>14</v>
       </c>
       <c r="B338" s="62" t="s">
+        <v>692</v>
+      </c>
+      <c r="C338" s="62" t="s">
         <v>693</v>
       </c>
-      <c r="C338" s="62" t="s">
+      <c r="D338" s="57" t="s">
         <v>694</v>
-      </c>
-      <c r="D338" s="57" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7058,13 +7058,13 @@
         <v>68</v>
       </c>
       <c r="B339" s="62" t="s">
+        <v>704</v>
+      </c>
+      <c r="C339" s="62" t="s">
         <v>705</v>
       </c>
-      <c r="C339" s="62" t="s">
+      <c r="D339" s="57" t="s">
         <v>706</v>
-      </c>
-      <c r="D339" s="57" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7072,13 +7072,13 @@
         <v>72</v>
       </c>
       <c r="B340" s="62" t="s">
+        <v>707</v>
+      </c>
+      <c r="C340" s="62" t="s">
         <v>708</v>
       </c>
-      <c r="C340" s="62" t="s">
+      <c r="D340" s="57" t="s">
         <v>709</v>
-      </c>
-      <c r="D340" s="57" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7086,41 +7086,41 @@
         <v>48</v>
       </c>
       <c r="B341" s="62" t="s">
+        <v>710</v>
+      </c>
+      <c r="C341" s="62" t="s">
         <v>711</v>
       </c>
-      <c r="C341" s="62" t="s">
+      <c r="D341" s="57" t="s">
         <v>712</v>
-      </c>
-      <c r="D341" s="57" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="62" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B342" s="62" t="s">
+        <v>713</v>
+      </c>
+      <c r="C342" s="62" t="s">
         <v>714</v>
       </c>
-      <c r="C342" s="62" t="s">
+      <c r="D342" s="57" t="s">
         <v>715</v>
-      </c>
-      <c r="D342" s="57" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="62" t="s">
+        <v>716</v>
+      </c>
+      <c r="B343" s="62" t="s">
         <v>717</v>
       </c>
-      <c r="B343" s="62" t="s">
+      <c r="C343" s="62" t="s">
         <v>718</v>
       </c>
-      <c r="C343" s="62" t="s">
+      <c r="D343" s="57" t="s">
         <v>719</v>
-      </c>
-      <c r="D343" s="57" t="s">
-        <v>720</v>
       </c>
     </row>
   </sheetData>
@@ -7171,9 +7171,10 @@
     <hyperlink ref="D66" r:id="rId41" xr:uid="{4ADFA047-8BEA-485C-9922-899E25E27867}"/>
     <hyperlink ref="D80" r:id="rId42" xr:uid="{9FA6E024-1E52-4D58-AE56-665DF705FF84}"/>
     <hyperlink ref="D319" r:id="rId43" xr:uid="{9D77423C-C774-4E73-80AC-8111A43E2E15}"/>
+    <hyperlink ref="D34" r:id="rId44" xr:uid="{9BC176C0-6381-4543-A209-397D4DBD321E}"/>
   </hyperlinks>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId44"/>
+  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId45"/>
   <rowBreaks count="6" manualBreakCount="6">
     <brk id="47" max="3" man="1"/>
     <brk id="88" max="3" man="1"/>
@@ -7182,6 +7183,6 @@
     <brk id="218" max="3" man="1"/>
     <brk id="264" max="3" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId45"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SW modified Musqueum Roster
</commit_message>
<xml_diff>
--- a/secure/club-roster2019.xlsx
+++ b/secure/club-roster2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C12613-F7F8-4626-BCB9-D7869E598978}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBDA31A-8413-48DE-9A9A-C3AC832499AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="540" windowWidth="22050" windowHeight="14265" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
+    <workbookView xWindow="2910" yWindow="2520" windowWidth="19920" windowHeight="11490" xr2:uid="{5FAFD24B-4FB2-4102-ACAF-F660D41EEEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="747">
   <si>
     <t>Beach Grove Golf Club</t>
   </si>
@@ -1090,15 +1090,6 @@
     <t>vjewison@icloud.com</t>
   </si>
   <si>
-    <t>Irena Bell</t>
-  </si>
-  <si>
-    <t>778-997-2602</t>
-  </si>
-  <si>
-    <t>irenabell@outlook.com</t>
-  </si>
-  <si>
     <t>Rosemary Dickenson</t>
   </si>
   <si>
@@ -2264,6 +2255,21 @@
   </si>
   <si>
     <t>macclogan@shaw.ca</t>
+  </si>
+  <si>
+    <t>Acting Vice Captain</t>
+  </si>
+  <si>
+    <t>Acting Handicap</t>
+  </si>
+  <si>
+    <t>Esther Yeoh</t>
+  </si>
+  <si>
+    <t>604-910-3346</t>
+  </si>
+  <si>
+    <t>eyeoh09@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -3114,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EEE842-FA9A-4617-9438-69514D1A7666}">
   <dimension ref="A1:F343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G177" sqref="G177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,7 +3135,7 @@
     <row r="1" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="67" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C1" s="68"/>
       <c r="D1"/>
@@ -3507,7 +3513,7 @@
         <v>77</v>
       </c>
       <c r="D34" s="65" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -3876,18 +3882,18 @@
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="26"/>
       <c r="B66" s="38" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="D66" s="66" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="5"/>
@@ -4048,7 +4054,7 @@
         <v>180</v>
       </c>
       <c r="D80" s="65" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -4697,25 +4703,25 @@
         <v>304</v>
       </c>
       <c r="B136" s="32" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C136" s="42" t="s">
         <v>305</v>
       </c>
       <c r="D136" s="33" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="26"/>
       <c r="B137" s="32" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C137" s="43">
         <v>0</v>
       </c>
       <c r="D137" s="33" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4723,10 +4729,10 @@
         <v>8</v>
       </c>
       <c r="B138" s="44" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C138" s="63" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="D138" s="53">
         <v>0</v>
@@ -4735,7 +4741,7 @@
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="50"/>
       <c r="B139" s="51" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C139" s="52"/>
       <c r="D139" s="54"/>
@@ -4743,7 +4749,7 @@
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="45"/>
       <c r="B140" s="46" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="C140" s="47"/>
       <c r="D140" s="48"/>
@@ -4777,11 +4783,11 @@
         <v>14</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C143" s="39"/>
       <c r="D143" s="33" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4789,16 +4795,16 @@
         <v>15</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C144" s="26"/>
       <c r="D144" s="33" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="26" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="B145" s="32"/>
       <c r="C145" s="26"/>
@@ -4811,11 +4817,11 @@
         <v>308</v>
       </c>
       <c r="B146" s="32" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C146" s="26"/>
       <c r="D146" s="33" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4823,11 +4829,11 @@
         <v>308</v>
       </c>
       <c r="B147" s="32" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C147" s="26"/>
       <c r="D147" s="33" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,7 +4866,7 @@
     </row>
     <row r="152" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="5"/>
@@ -5072,16 +5078,16 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="26" t="s">
-        <v>22</v>
+        <v>742</v>
       </c>
       <c r="B170" s="39" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="C170" s="39" t="s">
-        <v>354</v>
-      </c>
-      <c r="D170" s="56" t="s">
-        <v>355</v>
+        <v>362</v>
+      </c>
+      <c r="D170" s="65" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5089,11 +5095,11 @@
         <v>5</v>
       </c>
       <c r="B171" s="39" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C171" s="39"/>
       <c r="D171" s="56" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5101,13 +5107,13 @@
         <v>8</v>
       </c>
       <c r="B172" s="39" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C172" s="39" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D172" s="56" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5115,27 +5121,27 @@
         <v>11</v>
       </c>
       <c r="B173" s="39" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C173" s="39" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D173" s="56" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="26" t="s">
-        <v>14</v>
+        <v>743</v>
       </c>
       <c r="B174" s="39" t="s">
-        <v>364</v>
+        <v>744</v>
       </c>
       <c r="C174" s="39" t="s">
-        <v>365</v>
-      </c>
-      <c r="D174" s="56" t="s">
-        <v>366</v>
+        <v>745</v>
+      </c>
+      <c r="D174" s="65" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -5143,13 +5149,13 @@
         <v>48</v>
       </c>
       <c r="B175" s="39" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C175" s="39" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D175" s="36" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -5159,7 +5165,7 @@
     </row>
     <row r="177" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B177" s="2"/>
       <c r="D177" s="7"/>
@@ -5169,13 +5175,13 @@
         <v>1</v>
       </c>
       <c r="B178" s="26" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C178" s="26" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D178" s="27" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -5183,13 +5189,13 @@
         <v>22</v>
       </c>
       <c r="B179" s="26" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C179" s="26" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D179" s="27" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -5197,13 +5203,13 @@
         <v>5</v>
       </c>
       <c r="B180" s="26" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C180" s="26" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D180" s="27" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,13 +5217,13 @@
         <v>8</v>
       </c>
       <c r="B181" s="26" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C181" s="26" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D181" s="27" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,13 +5231,13 @@
         <v>11</v>
       </c>
       <c r="B182" s="26" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C182" s="26" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D182" s="27" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -5239,13 +5245,13 @@
         <v>14</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C183" s="26" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D183" s="28" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5255,7 +5261,7 @@
     </row>
     <row r="185" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="5"/>
@@ -5265,27 +5271,27 @@
         <v>1</v>
       </c>
       <c r="B186" s="26" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C186" s="26" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D186" s="27" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="B187" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="C187" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="D187" s="27" t="s">
         <v>393</v>
-      </c>
-      <c r="B187" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="C187" s="26" t="s">
-        <v>395</v>
-      </c>
-      <c r="D187" s="27" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,13 +5299,13 @@
         <v>5</v>
       </c>
       <c r="B188" s="26" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C188" s="26" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D188" s="27" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5307,13 +5313,13 @@
         <v>8</v>
       </c>
       <c r="B189" s="26" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C189" s="26" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D189" s="27" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5321,13 +5327,13 @@
         <v>11</v>
       </c>
       <c r="B190" s="26" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C190" s="26" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D190" s="27" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5335,13 +5341,13 @@
         <v>14</v>
       </c>
       <c r="B191" s="26" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C191" s="26" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D191" s="27" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5349,18 +5355,18 @@
         <v>48</v>
       </c>
       <c r="B192" s="26" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C192" s="26" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D192" s="27" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="5"/>
@@ -5370,13 +5376,13 @@
         <v>1</v>
       </c>
       <c r="B195" s="26" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C195" s="26" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D195" s="27" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5384,13 +5390,13 @@
         <v>22</v>
       </c>
       <c r="B196" s="26" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D196" s="27" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5398,13 +5404,13 @@
         <v>5</v>
       </c>
       <c r="B197" s="26" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C197" s="26" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D197" s="27" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5412,13 +5418,13 @@
         <v>8</v>
       </c>
       <c r="B198" s="26" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C198" s="26" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D198" s="27" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5426,18 +5432,18 @@
         <v>14</v>
       </c>
       <c r="B199" s="26" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C199" s="26" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D199" s="27" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="5"/>
@@ -5447,13 +5453,13 @@
         <v>1</v>
       </c>
       <c r="B202" s="26" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C202" s="26" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D202" s="27" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5461,13 +5467,13 @@
         <v>22</v>
       </c>
       <c r="B203" s="26" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C203" s="26" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D203" s="27" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5475,13 +5481,13 @@
         <v>5</v>
       </c>
       <c r="B204" s="26" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C204" s="26" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D204" s="27" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5489,13 +5495,13 @@
         <v>8</v>
       </c>
       <c r="B205" s="26" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C205" s="26" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D205" s="27" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5503,13 +5509,13 @@
         <v>11</v>
       </c>
       <c r="B206" s="26" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C206" s="26" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D206" s="27" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5517,13 +5523,13 @@
         <v>14</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C207" s="26" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D207" s="27" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5531,7 +5537,7 @@
     </row>
     <row r="209" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D209" s="7"/>
     </row>
@@ -5540,13 +5546,13 @@
         <v>1</v>
       </c>
       <c r="B210" s="26" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C210" s="26" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D210" s="27" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5554,13 +5560,13 @@
         <v>22</v>
       </c>
       <c r="B211" s="26" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C211" s="26" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D211" s="27" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5568,11 +5574,11 @@
         <v>5</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C212" s="26"/>
       <c r="D212" s="27" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5588,11 +5594,11 @@
         <v>14</v>
       </c>
       <c r="B214" s="26" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C214" s="26"/>
       <c r="D214" s="27" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5600,11 +5606,11 @@
         <v>15</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C215" s="26"/>
       <c r="D215" s="27" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5612,13 +5618,13 @@
         <v>68</v>
       </c>
       <c r="B216" s="26" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C216" s="26" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D216" s="27" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5626,13 +5632,13 @@
         <v>72</v>
       </c>
       <c r="B217" s="26" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C217" s="26" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D217" s="27" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5640,13 +5646,13 @@
         <v>48</v>
       </c>
       <c r="B218" s="26" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C218" s="26" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D218" s="27" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5655,7 +5661,7 @@
     </row>
     <row r="220" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D220" s="7"/>
     </row>
@@ -5664,13 +5670,13 @@
         <v>1</v>
       </c>
       <c r="B221" s="26" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C221" s="26" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D221" s="27" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5678,13 +5684,13 @@
         <v>22</v>
       </c>
       <c r="B222" s="26" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C222" s="26" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D222" s="27" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5692,13 +5698,13 @@
         <v>5</v>
       </c>
       <c r="B223" s="26" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C223" s="26" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D223" s="27" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5706,13 +5712,13 @@
         <v>8</v>
       </c>
       <c r="B224" s="26" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C224" s="26" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D224" s="27" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5720,13 +5726,13 @@
         <v>11</v>
       </c>
       <c r="B225" s="26" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C225" s="26" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D225" s="27" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5734,13 +5740,13 @@
         <v>14</v>
       </c>
       <c r="B226" s="26" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C226" s="26" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D226" s="27" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5748,13 +5754,13 @@
         <v>68</v>
       </c>
       <c r="B227" s="26" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C227" s="26" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D227" s="27" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5778,13 +5784,13 @@
         <v>106</v>
       </c>
       <c r="B230" s="26" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C230" s="26" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D230" s="57" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5792,7 +5798,7 @@
     </row>
     <row r="232" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B232" s="4"/>
       <c r="C232" s="5"/>
@@ -5802,13 +5808,13 @@
         <v>1</v>
       </c>
       <c r="B233" s="26" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C233" s="26" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D233" s="27" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5816,13 +5822,13 @@
         <v>22</v>
       </c>
       <c r="B234" s="26" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C234" s="26" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D234" s="27" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5830,13 +5836,13 @@
         <v>5</v>
       </c>
       <c r="B235" s="26" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C235" s="26" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D235" s="27" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5844,11 +5850,11 @@
         <v>8</v>
       </c>
       <c r="B236" s="26" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C236" s="26"/>
       <c r="D236" s="27" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5864,11 +5870,11 @@
         <v>14</v>
       </c>
       <c r="B238" s="26" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C238" s="26"/>
       <c r="D238" s="27" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -5876,11 +5882,11 @@
         <v>15</v>
       </c>
       <c r="B239" s="26" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C239" s="26"/>
       <c r="D239" s="27" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -5888,13 +5894,13 @@
         <v>68</v>
       </c>
       <c r="B240" s="26" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C240" s="26" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D240" s="27" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5902,13 +5908,13 @@
         <v>72</v>
       </c>
       <c r="B241" s="26" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C241" s="26" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D241" s="27" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5916,16 +5922,16 @@
         <v>48</v>
       </c>
       <c r="B242" s="26" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C242" s="26"/>
       <c r="D242" s="27" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="12" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="5"/>
@@ -5935,13 +5941,13 @@
         <v>1</v>
       </c>
       <c r="B245" s="58" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C245" s="58" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D245" s="59" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -5949,13 +5955,13 @@
         <v>22</v>
       </c>
       <c r="B246" s="26" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C246" s="26" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D246" s="27" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -5963,13 +5969,13 @@
         <v>5</v>
       </c>
       <c r="B247" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C247" s="26" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D247" s="28" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5977,13 +5983,13 @@
         <v>8</v>
       </c>
       <c r="B248" s="26" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C248" s="26" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D248" s="28" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -5991,13 +5997,13 @@
         <v>11</v>
       </c>
       <c r="B249" s="26" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C249" s="26" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D249" s="28" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -6005,13 +6011,13 @@
         <v>14</v>
       </c>
       <c r="B250" s="26" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C250" s="26" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D250" s="28" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -6019,18 +6025,18 @@
         <v>68</v>
       </c>
       <c r="B251" s="26" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C251" s="60" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D251" s="28" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="5"/>
@@ -6040,13 +6046,13 @@
         <v>1</v>
       </c>
       <c r="B254" s="26" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C254" s="26" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D254" s="27" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -6054,13 +6060,13 @@
         <v>22</v>
       </c>
       <c r="B255" s="26" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C255" s="26" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D255" s="27" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -6068,13 +6074,13 @@
         <v>5</v>
       </c>
       <c r="B256" s="26" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C256" s="26" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D256" s="27" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -6082,13 +6088,13 @@
         <v>8</v>
       </c>
       <c r="B257" s="26" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C257" s="26" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D257" s="27" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -6096,13 +6102,13 @@
         <v>11</v>
       </c>
       <c r="B258" s="26" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C258" s="26" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D258" s="27" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,13 +6116,13 @@
         <v>14</v>
       </c>
       <c r="B259" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C259" s="26" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D259" s="27" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -6124,13 +6130,13 @@
         <v>68</v>
       </c>
       <c r="B260" s="26" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C260" s="26" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D260" s="27" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
@@ -6138,13 +6144,13 @@
         <v>72</v>
       </c>
       <c r="B261" s="26" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C261" s="26" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D261" s="27" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -6152,13 +6158,13 @@
         <v>48</v>
       </c>
       <c r="B262" s="26" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C262" s="26" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D262" s="27" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
@@ -6166,32 +6172,32 @@
         <v>106</v>
       </c>
       <c r="B263" s="26" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C263" s="26" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D263" s="27" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="26" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B264" s="26" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C264" s="26" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D264" s="27" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="13" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B266" s="4"/>
       <c r="C266" s="5"/>
@@ -6201,13 +6207,13 @@
         <v>1</v>
       </c>
       <c r="B267" s="26" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C267" s="26" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D267" s="27" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,13 +6221,13 @@
         <v>22</v>
       </c>
       <c r="B268" s="26" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C268" s="26" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D268" s="27" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
@@ -6229,13 +6235,13 @@
         <v>5</v>
       </c>
       <c r="B269" s="26" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C269" s="26" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D269" s="27" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -6243,13 +6249,13 @@
         <v>8</v>
       </c>
       <c r="B270" s="26" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C270" s="26" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D270" s="27" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6257,13 +6263,13 @@
         <v>11</v>
       </c>
       <c r="B271" s="26" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C271" s="26" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D271" s="27" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -6271,13 +6277,13 @@
         <v>14</v>
       </c>
       <c r="B272" s="26" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C272" s="26" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D272" s="27" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -6285,13 +6291,13 @@
         <v>15</v>
       </c>
       <c r="B273" s="26" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C273" s="26" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D273" s="27" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6299,13 +6305,13 @@
         <v>72</v>
       </c>
       <c r="B274" s="26" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C274" s="26" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D274" s="27" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -6313,18 +6319,18 @@
         <v>48</v>
       </c>
       <c r="B275" s="26" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C275" s="26" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D275" s="27" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A277" s="13" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B277" s="4"/>
       <c r="C277" s="5"/>
@@ -6334,13 +6340,13 @@
         <v>1</v>
       </c>
       <c r="B278" s="26" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C278" s="26" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D278" s="61" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -6348,13 +6354,13 @@
         <v>22</v>
       </c>
       <c r="B279" s="26" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C279" s="26" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D279" s="61" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -6362,13 +6368,13 @@
         <v>5</v>
       </c>
       <c r="B280" s="26" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C280" s="26" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D280" s="28" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -6376,13 +6382,13 @@
         <v>8</v>
       </c>
       <c r="B281" s="26" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C281" s="26" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D281" s="61" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -6390,13 +6396,13 @@
         <v>11</v>
       </c>
       <c r="B282" s="26" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C282" s="26" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D282" s="28" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -6404,13 +6410,13 @@
         <v>14</v>
       </c>
       <c r="B283" s="26" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C283" s="26" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D283" s="28" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -6426,18 +6432,18 @@
         <v>48</v>
       </c>
       <c r="B285" s="26" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C285" s="26" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D285" s="61" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -6447,13 +6453,13 @@
         <v>1</v>
       </c>
       <c r="B288" s="26" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C288" s="26" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D288" s="27" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6461,13 +6467,13 @@
         <v>22</v>
       </c>
       <c r="B289" s="26" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C289" s="26" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D289" s="27" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6475,13 +6481,13 @@
         <v>5</v>
       </c>
       <c r="B290" s="26" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C290" s="26" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D290" s="27" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -6489,13 +6495,13 @@
         <v>8</v>
       </c>
       <c r="B291" s="26" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C291" s="26" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D291" s="27" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -6503,13 +6509,13 @@
         <v>11</v>
       </c>
       <c r="B292" s="26" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C292" s="26" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D292" s="27" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -6517,27 +6523,27 @@
         <v>14</v>
       </c>
       <c r="B293" s="26" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C293" s="26" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D293" s="27" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="26" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B294" s="26" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C294" s="26" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D294" s="27" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -6545,7 +6551,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="22" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B296" s="5"/>
       <c r="D296" s="7"/>
@@ -6555,13 +6561,13 @@
         <v>1</v>
       </c>
       <c r="B297" s="26" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C297" s="26" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D297" s="26" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.25">
@@ -6569,13 +6575,13 @@
         <v>22</v>
       </c>
       <c r="B298" s="26" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C298" s="26" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D298" s="26" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -6583,13 +6589,13 @@
         <v>5</v>
       </c>
       <c r="B299" s="26" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C299" s="26" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D299" s="26" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -6597,13 +6603,13 @@
         <v>8</v>
       </c>
       <c r="B300" s="26" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C300" s="26" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D300" s="26" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -6611,25 +6617,25 @@
         <v>11</v>
       </c>
       <c r="B301" s="26" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C301" s="26" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D301" s="26" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="302" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="26"/>
       <c r="B302" s="26" t="s">
+        <v>624</v>
+      </c>
+      <c r="C302" s="26" t="s">
         <v>627</v>
       </c>
-      <c r="C302" s="26" t="s">
-        <v>630</v>
-      </c>
       <c r="D302" s="26" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.25">
@@ -6637,7 +6643,7 @@
     </row>
     <row r="304" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A304" s="23" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
@@ -6647,13 +6653,13 @@
         <v>1</v>
       </c>
       <c r="B305" s="26" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C305" s="26" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D305" s="27" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -6661,13 +6667,13 @@
         <v>22</v>
       </c>
       <c r="B306" s="26" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C306" s="26" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D306" s="27" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -6675,13 +6681,13 @@
         <v>5</v>
       </c>
       <c r="B307" s="26" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C307" s="26" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D307" s="27" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -6689,13 +6695,13 @@
         <v>8</v>
       </c>
       <c r="B308" s="26" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C308" s="26" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D308" s="27" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -6703,13 +6709,13 @@
         <v>11</v>
       </c>
       <c r="B309" s="26" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C309" s="26" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D309" s="27" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -6717,13 +6723,13 @@
         <v>14</v>
       </c>
       <c r="B310" s="26" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C310" s="26" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D310" s="27" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.25">
@@ -6731,13 +6737,13 @@
         <v>68</v>
       </c>
       <c r="B311" s="26" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C311" s="26" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D311" s="27" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -6745,13 +6751,13 @@
         <v>72</v>
       </c>
       <c r="B312" s="26" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C312" s="26" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D312" s="27" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -6759,7 +6765,7 @@
     </row>
     <row r="314" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A314" s="8" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D314" s="21"/>
     </row>
@@ -6768,23 +6774,23 @@
         <v>1</v>
       </c>
       <c r="B315" s="26" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C315" s="26" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D315" s="27" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="26"/>
       <c r="B316" s="26" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C316" s="26"/>
       <c r="D316" s="27" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.25">
@@ -6792,13 +6798,13 @@
         <v>22</v>
       </c>
       <c r="B317" s="26" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C317" s="26" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D317" s="27" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -6806,13 +6812,13 @@
         <v>5</v>
       </c>
       <c r="B318" s="26" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C318" s="26" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D318" s="27" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -6820,13 +6826,13 @@
         <v>8</v>
       </c>
       <c r="B319" s="26" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="C319" s="26" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D319" s="61" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -6834,13 +6840,13 @@
         <v>11</v>
       </c>
       <c r="B320" s="26" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C320" s="26" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="D320" s="27" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -6848,18 +6854,18 @@
         <v>14</v>
       </c>
       <c r="B321" s="26" t="s">
+        <v>665</v>
+      </c>
+      <c r="C321" s="26" t="s">
         <v>668</v>
       </c>
-      <c r="C321" s="26" t="s">
-        <v>671</v>
-      </c>
       <c r="D321" s="27" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A323" s="13" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B323" s="4"/>
       <c r="C323" s="5"/>
@@ -6869,13 +6875,13 @@
         <v>1</v>
       </c>
       <c r="B324" s="26" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C324" s="26" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D324" s="27" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -6883,13 +6889,13 @@
         <v>5</v>
       </c>
       <c r="B325" s="26" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C325" s="26" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D325" s="27" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -6897,13 +6903,13 @@
         <v>8</v>
       </c>
       <c r="B326" s="26" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C326" s="26" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D326" s="27" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -6911,13 +6917,13 @@
         <v>11</v>
       </c>
       <c r="B327" s="26" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C327" s="26" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D327" s="27" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6925,13 +6931,13 @@
         <v>14</v>
       </c>
       <c r="B328" s="26" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C328" s="26" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D328" s="27" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -6939,13 +6945,13 @@
         <v>68</v>
       </c>
       <c r="B329" s="26" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C329" s="26" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D329" s="27" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -6953,18 +6959,18 @@
         <v>72</v>
       </c>
       <c r="B330" s="26" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="C330" s="26" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D330" s="27" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="332" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A332" s="13" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="B332" s="24"/>
       <c r="C332" s="25"/>
@@ -6974,13 +6980,13 @@
         <v>1</v>
       </c>
       <c r="B333" s="62" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C333" s="62" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D333" s="57" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -6988,13 +6994,13 @@
         <v>22</v>
       </c>
       <c r="B334" s="62" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C334" s="62" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D334" s="57" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -7002,13 +7008,13 @@
         <v>5</v>
       </c>
       <c r="B335" s="62" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C335" s="62" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D335" s="57" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -7016,13 +7022,13 @@
         <v>8</v>
       </c>
       <c r="B336" s="62" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="C336" s="62" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D336" s="57" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -7030,13 +7036,13 @@
         <v>11</v>
       </c>
       <c r="B337" s="62" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C337" s="62" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D337" s="57" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -7044,13 +7050,13 @@
         <v>14</v>
       </c>
       <c r="B338" s="62" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C338" s="62" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D338" s="57" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7058,13 +7064,13 @@
         <v>68</v>
       </c>
       <c r="B339" s="62" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C339" s="62" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D339" s="57" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7072,13 +7078,13 @@
         <v>72</v>
       </c>
       <c r="B340" s="62" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C340" s="62" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D340" s="57" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7086,13 +7092,13 @@
         <v>48</v>
       </c>
       <c r="B341" s="62" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C341" s="62" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D341" s="57" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -7100,27 +7106,27 @@
         <v>308</v>
       </c>
       <c r="B342" s="62" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="C342" s="62" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="D342" s="57" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="62" t="s">
+        <v>713</v>
+      </c>
+      <c r="B343" s="62" t="s">
+        <v>714</v>
+      </c>
+      <c r="C343" s="62" t="s">
+        <v>715</v>
+      </c>
+      <c r="D343" s="57" t="s">
         <v>716</v>
-      </c>
-      <c r="B343" s="62" t="s">
-        <v>717</v>
-      </c>
-      <c r="C343" s="62" t="s">
-        <v>718</v>
-      </c>
-      <c r="D343" s="57" t="s">
-        <v>719</v>
       </c>
     </row>
   </sheetData>
@@ -7172,9 +7178,11 @@
     <hyperlink ref="D80" r:id="rId42" xr:uid="{9FA6E024-1E52-4D58-AE56-665DF705FF84}"/>
     <hyperlink ref="D319" r:id="rId43" xr:uid="{9D77423C-C774-4E73-80AC-8111A43E2E15}"/>
     <hyperlink ref="D34" r:id="rId44" xr:uid="{9BC176C0-6381-4543-A209-397D4DBD321E}"/>
+    <hyperlink ref="D174" r:id="rId45" xr:uid="{AD4F5725-D065-4CB9-A418-0BE9DEE83A18}"/>
+    <hyperlink ref="D170" r:id="rId46" xr:uid="{FE8A8F89-2F8F-46FF-AEC7-D545F1BD6B5A}"/>
   </hyperlinks>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId45"/>
+  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId47"/>
   <rowBreaks count="6" manualBreakCount="6">
     <brk id="47" max="3" man="1"/>
     <brk id="88" max="3" man="1"/>
@@ -7183,6 +7191,6 @@
     <brk id="218" max="3" man="1"/>
     <brk id="264" max="3" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId46"/>
+  <drawing r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>